<commit_message>
signup as child company
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,37 +9,38 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
     <sheet name="LoginData" sheetId="2" r:id="rId2"/>
     <sheet name="SignupChildComp" sheetId="30" r:id="rId3"/>
-    <sheet name="ConfigAccType" sheetId="3" r:id="rId4"/>
-    <sheet name="EditConfigAccType" sheetId="4" r:id="rId5"/>
-    <sheet name="ConfigPaymentMethod" sheetId="5" r:id="rId6"/>
-    <sheet name="ConfigPaymentMethCredit" sheetId="6" r:id="rId7"/>
-    <sheet name="ConfigOrderPeriods" sheetId="7" r:id="rId8"/>
-    <sheet name="ConfigCollection" sheetId="8" r:id="rId9"/>
-    <sheet name="ConfigBillingProcess" sheetId="9" r:id="rId10"/>
-    <sheet name="ConfigNewInfoType" sheetId="10" r:id="rId11"/>
-    <sheet name="AddEditCategory" sheetId="11" r:id="rId12"/>
-    <sheet name="AddProduct" sheetId="12" r:id="rId13"/>
-    <sheet name="AddCustomer" sheetId="13" r:id="rId14"/>
-    <sheet name="CustOrder" sheetId="14" r:id="rId15"/>
-    <sheet name="OrderHierarcy" sheetId="16" r:id="rId16"/>
-    <sheet name="Agent" sheetId="17" r:id="rId17"/>
-    <sheet name="AgentPlugin" sheetId="18" r:id="rId18"/>
-    <sheet name="AgentComProcess" sheetId="19" r:id="rId19"/>
-    <sheet name="Reports" sheetId="20" r:id="rId20"/>
-    <sheet name="MakePayment" sheetId="21" r:id="rId21"/>
-    <sheet name="CreatingOrders" sheetId="23" r:id="rId22"/>
-    <sheet name="Billing" sheetId="24" r:id="rId23"/>
-    <sheet name="Collections" sheetId="25" r:id="rId24"/>
-    <sheet name="TearDown" sheetId="26" r:id="rId25"/>
-    <sheet name="Discount" sheetId="27" r:id="rId26"/>
-    <sheet name="AddingAsset" sheetId="28" r:id="rId27"/>
-    <sheet name="Mediation" sheetId="29" r:id="rId28"/>
+    <sheet name="SignupChildCompInvoice" sheetId="31" r:id="rId4"/>
+    <sheet name="ConfigAccType" sheetId="3" r:id="rId5"/>
+    <sheet name="EditConfigAccType" sheetId="4" r:id="rId6"/>
+    <sheet name="ConfigPaymentMethod" sheetId="5" r:id="rId7"/>
+    <sheet name="ConfigPaymentMethCredit" sheetId="6" r:id="rId8"/>
+    <sheet name="ConfigOrderPeriods" sheetId="7" r:id="rId9"/>
+    <sheet name="ConfigCollection" sheetId="8" r:id="rId10"/>
+    <sheet name="ConfigBillingProcess" sheetId="9" r:id="rId11"/>
+    <sheet name="ConfigNewInfoType" sheetId="10" r:id="rId12"/>
+    <sheet name="AddEditCategory" sheetId="11" r:id="rId13"/>
+    <sheet name="AddProduct" sheetId="12" r:id="rId14"/>
+    <sheet name="AddCustomer" sheetId="13" r:id="rId15"/>
+    <sheet name="CustOrder" sheetId="14" r:id="rId16"/>
+    <sheet name="OrderHierarcy" sheetId="16" r:id="rId17"/>
+    <sheet name="Agent" sheetId="17" r:id="rId18"/>
+    <sheet name="AgentPlugin" sheetId="18" r:id="rId19"/>
+    <sheet name="AgentComProcess" sheetId="19" r:id="rId20"/>
+    <sheet name="Reports" sheetId="20" r:id="rId21"/>
+    <sheet name="MakePayment" sheetId="21" r:id="rId22"/>
+    <sheet name="CreatingOrders" sheetId="23" r:id="rId23"/>
+    <sheet name="Billing" sheetId="24" r:id="rId24"/>
+    <sheet name="Collections" sheetId="25" r:id="rId25"/>
+    <sheet name="TearDown" sheetId="26" r:id="rId26"/>
+    <sheet name="Discount" sheetId="27" r:id="rId27"/>
+    <sheet name="AddingAsset" sheetId="28" r:id="rId28"/>
+    <sheet name="Mediation" sheetId="29" r:id="rId29"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="109">
   <si>
     <t>indianashu@gmail.com</t>
   </si>
@@ -718,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -788,6 +789,50 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -821,7 +866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -856,7 +901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -903,7 +948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -968,7 +1013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
@@ -1033,7 +1078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
@@ -1092,7 +1137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
@@ -1163,7 +1208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
@@ -1234,7 +1279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -1259,44 +1304,6 @@
       </c>
       <c r="E1">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1339,6 +1346,44 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1405,7 +1450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -1452,7 +1497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK1"/>
   <sheetViews>
@@ -1580,7 +1625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -1633,7 +1678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -1710,7 +1755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1748,7 +1793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1792,7 +1837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -1848,7 +1893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -1926,7 +1971,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:W1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2006,6 +2053,88 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1">
+        <v>91</v>
+      </c>
+      <c r="I1">
+        <v>98452</v>
+      </c>
+      <c r="J1">
+        <v>50449</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1">
+        <v>560035</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O1" r:id="rId1" display="indianashu@gmail.com"/>
+    <hyperlink ref="K1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2042,7 +2171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -2080,7 +2209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2115,7 +2244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2150,7 +2279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2183,48 +2312,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated xpath for configurations menu
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2637,8 +2637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
xpath changes for agent commissions pages
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="14" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="139">
   <si>
     <t>indianashu@gmail.com</t>
   </si>
@@ -471,6 +471,12 @@
   </si>
   <si>
     <t>sandhal</t>
+  </si>
+  <si>
+    <t>Agent A</t>
+  </si>
+  <si>
+    <t>Customer B</t>
   </si>
 </sst>
 </file>
@@ -1625,7 +1631,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1696,7 +1702,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1725,15 +1731,15 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1744,16 +1750,25 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
         <v>53</v>
       </c>
-      <c r="G1">
-        <v>2</v>
+      <c r="J1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2637,7 +2652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated xpath for addingasset page
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="14" activeTab="24"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="20" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -1733,7 +1733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -2279,8 +2279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated xpath for billingpage
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="20" activeTab="32"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="20" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <sheet name="AgentComProcess" sheetId="19" r:id="rId25"/>
     <sheet name="Reports" sheetId="20" r:id="rId26"/>
     <sheet name="MakePayment" sheetId="21" r:id="rId27"/>
-    <sheet name="CreatingOrders" sheetId="23" r:id="rId28"/>
+    <sheet name="BillingCreateOrders" sheetId="23" r:id="rId28"/>
     <sheet name="Billing" sheetId="24" r:id="rId29"/>
     <sheet name="Collections" sheetId="25" r:id="rId30"/>
     <sheet name="TearDown" sheetId="26" r:id="rId31"/>
@@ -1896,7 +1896,7 @@
   <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2023,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2279,7 +2279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change of xpath and image verification
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="20" activeTab="28"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -30,22 +30,23 @@
     <sheet name="AddProduct" sheetId="12" r:id="rId16"/>
     <sheet name="AddProductWithAsset" sheetId="32" r:id="rId17"/>
     <sheet name="AddCustomer" sheetId="13" r:id="rId18"/>
-    <sheet name="CustOrder" sheetId="14" r:id="rId19"/>
-    <sheet name="GenerateInvoice" sheetId="33" r:id="rId20"/>
-    <sheet name="GeneratePayInvoice" sheetId="34" r:id="rId21"/>
-    <sheet name="OrderHierarcy" sheetId="16" r:id="rId22"/>
-    <sheet name="Agent" sheetId="17" r:id="rId23"/>
-    <sheet name="AgentPlugin" sheetId="18" r:id="rId24"/>
-    <sheet name="AgentComProcess" sheetId="19" r:id="rId25"/>
-    <sheet name="Reports" sheetId="20" r:id="rId26"/>
-    <sheet name="MakePayment" sheetId="21" r:id="rId27"/>
-    <sheet name="BillingCreateOrders" sheetId="23" r:id="rId28"/>
-    <sheet name="Billing" sheetId="24" r:id="rId29"/>
-    <sheet name="Collections" sheetId="25" r:id="rId30"/>
-    <sheet name="TearDown" sheetId="26" r:id="rId31"/>
-    <sheet name="Discount" sheetId="27" r:id="rId32"/>
-    <sheet name="AddingAsset" sheetId="28" r:id="rId33"/>
-    <sheet name="Mediation" sheetId="29" r:id="rId34"/>
+    <sheet name="AddCustomerChild" sheetId="37" r:id="rId19"/>
+    <sheet name="CustOrder" sheetId="14" r:id="rId20"/>
+    <sheet name="GenerateInvoice" sheetId="33" r:id="rId21"/>
+    <sheet name="GeneratePayInvoice" sheetId="34" r:id="rId22"/>
+    <sheet name="OrderHierarcy" sheetId="16" r:id="rId23"/>
+    <sheet name="Agent" sheetId="17" r:id="rId24"/>
+    <sheet name="AgentPlugin" sheetId="18" r:id="rId25"/>
+    <sheet name="AgentComProcess" sheetId="19" r:id="rId26"/>
+    <sheet name="Reports" sheetId="20" r:id="rId27"/>
+    <sheet name="MakePayment" sheetId="21" r:id="rId28"/>
+    <sheet name="BillingCreateOrders" sheetId="23" r:id="rId29"/>
+    <sheet name="Billing" sheetId="24" r:id="rId30"/>
+    <sheet name="Collections" sheetId="25" r:id="rId31"/>
+    <sheet name="TearDown" sheetId="26" r:id="rId32"/>
+    <sheet name="Discount" sheetId="27" r:id="rId33"/>
+    <sheet name="AddingAsset" sheetId="28" r:id="rId34"/>
+    <sheet name="Mediation" sheetId="29" r:id="rId35"/>
   </sheets>
   <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="142">
   <si>
     <t>indianashu@gmail.com</t>
   </si>
@@ -152,9 +153,6 @@
     <t>Test Abc1</t>
   </si>
   <si>
-    <t>testadmin1</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -191,9 +189,6 @@
     <t>visa</t>
   </si>
   <si>
-    <t>abc kumar</t>
-  </si>
-  <si>
     <t>Agent1</t>
   </si>
   <si>
@@ -477,6 +472,21 @@
   </si>
   <si>
     <t>Customer B</t>
+  </si>
+  <si>
+    <t>Ashish</t>
+  </si>
+  <si>
+    <t>bsmith@abc.com</t>
+  </si>
+  <si>
+    <t>swilson@abc.com</t>
+  </si>
+  <si>
+    <t>22 Brian Smith</t>
+  </si>
+  <si>
+    <t>user-23</t>
   </si>
 </sst>
 </file>
@@ -820,13 +830,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" t="s">
         <v>131</v>
       </c>
-      <c r="C1" t="s">
-        <v>136</v>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
       </c>
       <c r="D1">
         <v>91</v>
@@ -841,13 +851,13 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -862,13 +872,13 @@
         <v>2</v>
       </c>
       <c r="O1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P1">
         <v>560035</v>
       </c>
       <c r="Q1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -989,13 +999,13 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K1">
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M1">
         <v>8</v>
@@ -1215,19 +1225,19 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
         <v>111</v>
-      </c>
-      <c r="E1">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" t="s">
-        <v>113</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -1239,17 +1249,17 @@
         <v>2</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" t="s">
         <v>114</v>
       </c>
-      <c r="N1" t="s">
-        <v>115</v>
-      </c>
-      <c r="O1" t="s">
-        <v>116</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1261,12 +1271,12 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -1286,31 +1296,31 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
-        <v>42</v>
-      </c>
       <c r="L1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1">
-        <v>4111111111111110</v>
+        <v>137</v>
+      </c>
+      <c r="M1" s="6">
+        <v>4111111111111150</v>
       </c>
       <c r="N1" s="4">
-        <v>44105</v>
+        <v>43862</v>
       </c>
     </row>
   </sheetData>
@@ -1323,15 +1333,18 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1348,34 +1361,43 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" t="s">
-        <v>35</v>
+        <v>125</v>
+      </c>
+      <c r="J1" s="6">
+        <v>4111111111111110</v>
+      </c>
+      <c r="K1" s="4">
+        <v>43862</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1">
-        <v>4</v>
-      </c>
-      <c r="N1">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
+        <v>124</v>
+      </c>
+      <c r="M1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1415,6 +1437,65 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1">
+        <v>4</v>
+      </c>
+      <c r="N1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1440,40 +1521,40 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
       <c r="L1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N1">
         <v>4</v>
       </c>
       <c r="O1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" t="s">
         <v>121</v>
-      </c>
-      <c r="P1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>123</v>
       </c>
       <c r="R1">
         <v>5</v>
@@ -1487,7 +1568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
@@ -1511,22 +1592,22 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J1">
         <v>500</v>
@@ -1538,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="M1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N1" s="6">
         <v>4111111111111150</v>
@@ -1552,7 +1633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -1573,60 +1654,60 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
         <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
       </c>
       <c r="G1">
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J1">
         <v>10</v>
       </c>
       <c r="K1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" t="s">
         <v>94</v>
       </c>
-      <c r="L1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>92</v>
-      </c>
-      <c r="R1" t="s">
-        <v>96</v>
-      </c>
       <c r="S1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
@@ -1647,16 +1728,16 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -1665,19 +1746,19 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K1">
         <v>12</v>
       </c>
       <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
         <v>49</v>
-      </c>
-      <c r="M1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" t="s">
-        <v>51</v>
       </c>
       <c r="O1">
         <v>5</v>
@@ -1697,7 +1778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -1718,7 +1799,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -1729,7 +1810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -1750,22 +1831,22 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J1">
         <v>1</v>
@@ -1776,7 +1857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -1806,13 +1887,13 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1">
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I1">
         <v>4111111111111110</v>
@@ -1824,27 +1905,27 @@
         <v>42379</v>
       </c>
       <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>58</v>
       </c>
-      <c r="O1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -1871,7 +1952,7 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G1">
         <v>4111111111111110</v>
@@ -1880,7 +1961,7 @@
         <v>44166</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J1" s="5">
         <v>10</v>
@@ -1891,7 +1972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK1"/>
   <sheetViews>
@@ -1918,10 +1999,10 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1">
         <v>1</v>
@@ -1930,7 +2011,7 @@
         <v>36892</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K1">
         <v>15</v>
@@ -1939,13 +2020,13 @@
         <v>36892</v>
       </c>
       <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" t="s">
         <v>63</v>
-      </c>
-      <c r="N1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" t="s">
-        <v>65</v>
       </c>
       <c r="P1" s="3">
         <v>36892</v>
@@ -1954,10 +2035,10 @@
         <v>20</v>
       </c>
       <c r="R1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T1" s="3">
         <v>36892</v>
@@ -1966,10 +2047,10 @@
         <v>5</v>
       </c>
       <c r="V1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="W1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X1" s="3">
         <v>36892</v>
@@ -1981,10 +2062,10 @@
         <v>14</v>
       </c>
       <c r="AA1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC1" s="3">
         <v>36892</v>
@@ -1996,10 +2077,10 @@
         <v>3</v>
       </c>
       <c r="AF1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AG1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AH1" s="3">
         <v>36892</v>
@@ -2019,11 +2100,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2046,22 +2156,22 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
         <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>72</v>
       </c>
       <c r="J1" s="3">
         <v>36893</v>
       </c>
       <c r="K1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L1" s="3">
         <v>36894</v>
@@ -2072,36 +2182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -2125,13 +2206,13 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G1" s="6">
         <v>411111111111111</v>
@@ -2146,22 +2227,22 @@
         <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L1">
         <v>42</v>
       </c>
       <c r="M1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O1" t="s">
         <v>18</v>
       </c>
       <c r="P1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q1" t="s">
         <v>19</v>
@@ -2170,15 +2251,15 @@
         <v>37015</v>
       </c>
       <c r="S1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -2199,26 +2280,26 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
@@ -2226,7 +2307,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2237,101 +2318,104 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
         <v>80</v>
       </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1">
+        <v>604</v>
+      </c>
+      <c r="O1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="G1">
-        <v>5</v>
+      <c r="G1" t="s">
+        <v>30</v>
       </c>
       <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
       <c r="I1" s="3">
         <v>42690</v>
       </c>
       <c r="J1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>86</v>
       </c>
-      <c r="L1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -2352,25 +2436,25 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>100</v>
-      </c>
-      <c r="I1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" t="s">
-        <v>102</v>
       </c>
       <c r="K1">
         <v>1</v>
@@ -2379,7 +2463,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N1">
         <v>1</v>
@@ -2391,10 +2475,10 @@
         <v>8</v>
       </c>
       <c r="Q1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="S1">
         <v>1</v>
@@ -2426,19 +2510,19 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" t="s">
         <v>128</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
         <v>129</v>
-      </c>
-      <c r="F1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2470,13 +2554,13 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
       </c>
       <c r="H1">
         <v>91</v>
@@ -2491,13 +2575,13 @@
         <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>3</v>
@@ -2512,13 +2596,13 @@
         <v>2</v>
       </c>
       <c r="S1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T1">
         <v>560035</v>
       </c>
       <c r="U1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2552,13 +2636,13 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
       </c>
       <c r="H1">
         <v>91</v>
@@ -2573,13 +2657,13 @@
         <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>3</v>
@@ -2594,13 +2678,13 @@
         <v>2</v>
       </c>
       <c r="S1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T1">
         <v>560035</v>
       </c>
       <c r="U1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed xpath for testcases
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="16" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="145">
   <si>
     <t>indianashu@gmail.com</t>
   </si>
@@ -417,9 +417,6 @@
     <t>Plan Product</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>Test Code</t>
   </si>
   <si>
@@ -487,6 +484,18 @@
   </si>
   <si>
     <t>user-23</t>
+  </si>
+  <si>
+    <t>22 - Brian Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer 22 receives invoices. </t>
+  </si>
+  <si>
+    <t>Product Code1 Description</t>
+  </si>
+  <si>
+    <t>Commission Product</t>
   </si>
 </sst>
 </file>
@@ -830,13 +839,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" t="s">
-        <v>134</v>
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
       </c>
       <c r="D1">
         <v>91</v>
@@ -857,7 +866,7 @@
         <v>105</v>
       </c>
       <c r="J1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -878,7 +887,7 @@
         <v>560035</v>
       </c>
       <c r="Q1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1296,7 +1305,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G1" t="s">
         <v>30</v>
@@ -1314,7 +1323,7 @@
         <v>41</v>
       </c>
       <c r="L1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M1" s="6">
         <v>4111111111111150</v>
@@ -1333,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,7 +1353,7 @@
     <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1361,16 +1370,16 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H1" t="s">
         <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J1" s="6">
         <v>4111111111111110</v>
@@ -1379,19 +1388,25 @@
         <v>43862</v>
       </c>
       <c r="L1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" t="s">
         <v>139</v>
-      </c>
-      <c r="N1" t="s">
-        <v>140</v>
       </c>
       <c r="O1">
         <v>22</v>
       </c>
       <c r="P1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" t="s">
         <v>141</v>
+      </c>
+      <c r="R1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1496,15 +1511,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1515,51 +1530,39 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>143</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="J1">
+        <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="L1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M1" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="N1">
-        <v>4</v>
-      </c>
-      <c r="O1" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>121</v>
-      </c>
-      <c r="R1">
-        <v>5</v>
-      </c>
-      <c r="S1">
+        <v>5</v>
+      </c>
+      <c r="O1">
         <v>10</v>
       </c>
     </row>
@@ -1592,7 +1595,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
         <v>30</v>
@@ -1601,10 +1604,10 @@
         <v>33</v>
       </c>
       <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
         <v>122</v>
-      </c>
-      <c r="H1" t="s">
-        <v>123</v>
       </c>
       <c r="I1" t="s">
         <v>67</v>
@@ -1619,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="M1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N1" s="6">
         <v>4111111111111150</v>
@@ -1831,10 +1834,10 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" t="s">
-        <v>136</v>
       </c>
       <c r="F1" t="s">
         <v>30</v>
@@ -1859,10 +1862,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1870,7 +1873,7 @@
     <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1919,6 +1922,9 @@
       <c r="P1" t="s">
         <v>58</v>
       </c>
+      <c r="Q1" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2121,7 +2127,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2345,13 +2351,13 @@
         <v>117</v>
       </c>
       <c r="M1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N1">
         <v>604</v>
       </c>
       <c r="O1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2510,19 +2516,19 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>127</v>
-      </c>
-      <c r="F1" t="s">
-        <v>128</v>
       </c>
       <c r="G1" t="s">
         <v>84</v>
       </c>
       <c r="H1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased the waitclass value
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="16" activeTab="26"/>
+    <workbookView xWindow="440" yWindow="800" windowWidth="28640" windowHeight="17540" tabRatio="500" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="146">
   <si>
     <t>indianashu@gmail.com</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t>Commission Product</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,8 +1095,8 @@
       <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
+      <c r="F1" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +1867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More changes done for correct data
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="622" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="148">
   <si>
     <t>test1234</t>
   </si>
@@ -186,6 +186,9 @@
     <t>New Test Category1</t>
   </si>
   <si>
+    <t>Asset Category1</t>
+  </si>
+  <si>
     <t>Available</t>
   </si>
   <si>
@@ -195,21 +198,24 @@
     <t>Tax ID</t>
   </si>
   <si>
-    <t>Test Abc</t>
+    <t>Product Code1 Description</t>
+  </si>
+  <si>
+    <t>'10/11/2016'</t>
   </si>
   <si>
     <t>United States Dollar</t>
   </si>
   <si>
+    <t>'01/01/2002'</t>
+  </si>
+  <si>
     <t>Test Abc1</t>
   </si>
   <si>
     <t>com.sapienter.jbilling.server.item.tasks.AssetUpdatedTask</t>
   </si>
   <si>
-    <t>Asset Category1</t>
-  </si>
-  <si>
     <t>Sim Cards</t>
   </si>
   <si>
@@ -261,7 +267,7 @@
     <t>22 - Brian Smith</t>
   </si>
   <si>
-    <t>Customer 22 receives invoices. </t>
+    <t>Customer 22 receives invoices.</t>
   </si>
   <si>
     <t>Customer A</t>
@@ -273,9 +279,6 @@
     <t>10/17/2016</t>
   </si>
   <si>
-    <t>Product Code1 Description</t>
-  </si>
-  <si>
     <t>Test Code</t>
   </si>
   <si>
@@ -453,7 +456,7 @@
     <t>Plan Product</t>
   </si>
   <si>
-    <t>Total = US$495.00            </t>
+    <t>Total = US$495.00</t>
   </si>
   <si>
     <t>Asset Customer</t>
@@ -948,8 +951,8 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1037,13 +1040,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.5296296296296"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3333333333333"/>
@@ -1052,7 +1055,7 @@
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>13</v>
       </c>
@@ -1080,6 +1083,9 @@
       <c r="I1" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1099,8 +1105,8 @@
   </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1119,43 +1125,43 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="n">
-        <v>42684</v>
+      <c r="G1" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="K1" s="3" t="n">
-        <v>42561</v>
+      <c r="K1" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1196,25 +1202,25 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>2</v>
@@ -1223,13 +1229,13 @@
         <v>19</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1278,25 +1284,25 @@
         <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="M1" s="4" t="n">
         <v>4111111111111150</v>
@@ -1354,16 +1360,16 @@
         <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="I1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J1" s="4" t="n">
         <v>4111111111111110</v>
@@ -1372,25 +1378,25 @@
         <v>43862</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>22</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1484,25 +1490,25 @@
         <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>4</v>
@@ -1549,34 +1555,34 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>4</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>5</v>
@@ -1625,22 +1631,22 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>500</v>
@@ -1652,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N1" s="4" t="n">
         <v>4111111111111150</v>
@@ -1699,52 +1705,52 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1785,16 +1791,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>15</v>
@@ -1803,19 +1809,19 @@
         <v>25</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -1868,7 +1874,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -1912,22 +1918,22 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
@@ -1979,13 +1985,13 @@
         <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>10</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>4111111111111110</v>
@@ -1997,22 +2003,22 @@
         <v>42379</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2059,7 +2065,7 @@
         <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>4111111111111110</v>
@@ -2068,7 +2074,7 @@
         <v>44166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J1" s="6" t="n">
         <v>10</v>
@@ -2118,10 +2124,10 @@
         <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
@@ -2130,7 +2136,7 @@
         <v>36892</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>15</v>
@@ -2139,13 +2145,13 @@
         <v>36892</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P1" s="3" t="n">
         <v>36892</v>
@@ -2154,10 +2160,10 @@
         <v>20</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T1" s="3" t="n">
         <v>36892</v>
@@ -2166,10 +2172,10 @@
         <v>5</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X1" s="3" t="n">
         <v>36892</v>
@@ -2181,10 +2187,10 @@
         <v>14</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AC1" s="3" t="n">
         <v>36892</v>
@@ -2196,10 +2202,10 @@
         <v>3</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AH1" s="3" t="n">
         <v>36892</v>
@@ -2299,22 +2305,22 @@
         <v>2</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J1" s="3" t="n">
         <v>36893</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L1" s="3" t="n">
         <v>36894</v>
@@ -2360,13 +2366,13 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G1" s="4" t="n">
         <v>411111111111111</v>
@@ -2381,22 +2387,22 @@
         <v>41</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>42</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>36</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>37</v>
@@ -2405,7 +2411,7 @@
         <v>37015</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2446,16 +2452,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2496,40 +2502,40 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>604</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2576,28 +2582,28 @@
         <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I1" s="3" t="n">
         <v>42690</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>19</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2638,25 +2644,25 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>1</v>
@@ -2665,7 +2671,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>1</v>
@@ -2677,10 +2683,10 @@
         <v>25</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
increased the waitsleep value
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25080" windowHeight="15700" tabRatio="622" firstSheet="11" activeTab="17"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="622" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
added signup child company scenarios
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="622" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="622" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="161">
   <si>
     <t>test1234</t>
   </si>
@@ -124,21 +124,6 @@
     <t>SIM-001</t>
   </si>
   <si>
-    <t>admin2</t>
-  </si>
-  <si>
-    <t>anilk</t>
-  </si>
-  <si>
-    <t>ppk</t>
-  </si>
-  <si>
-    <t>Design Ltd</t>
-  </si>
-  <si>
-    <t>Successfully created Design Ltd. You can now login with the username admin2 after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
     <t>Direct Customer</t>
   </si>
   <si>
@@ -521,6 +506,45 @@
   </si>
   <si>
     <t>Test Copy Product</t>
+  </si>
+  <si>
+    <t>Kauffman</t>
+  </si>
+  <si>
+    <t>Marta</t>
+  </si>
+  <si>
+    <t>marta@weddatatech.in</t>
+  </si>
+  <si>
+    <t>Web Data US Child</t>
+  </si>
+  <si>
+    <t>H-50</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Successfully created Web Data US Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>S.Bright</t>
+  </si>
+  <si>
+    <t>kevin@weddatatech.in</t>
+  </si>
+  <si>
+    <t>Web Data US Reseller</t>
+  </si>
+  <si>
+    <t>Successfully created Web Data US Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
 </sst>
 </file>
@@ -1017,13 +1041,13 @@
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1053,10 +1077,10 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F1">
         <v>1</v>
@@ -1089,31 +1113,31 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E1">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G1">
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I1">
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="K1">
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="M1">
         <v>8</v>
@@ -1152,7 +1176,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -1185,13 +1209,13 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1204,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -1221,25 +1245,25 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1269,49 +1293,49 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
         <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L1">
         <v>500</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N1" t="s">
         <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="P1">
         <v>50</v>
       </c>
       <c r="Q1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="R1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S1" t="s">
         <v>15</v>
@@ -1320,10 +1344,10 @@
         <v>10</v>
       </c>
       <c r="U1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="V1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1353,25 +1377,25 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
         <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K1">
         <v>50</v>
@@ -1404,25 +1428,25 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E1">
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K1">
         <v>2</v>
@@ -1431,13 +1455,13 @@
         <v>19</v>
       </c>
       <c r="M1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1468,28 +1492,28 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="M1" s="4">
         <v>4111111111111150</v>
@@ -1561,19 +1585,19 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J1" s="4">
         <v>4111111111111110</v>
@@ -1582,25 +1606,25 @@
         <v>43862</v>
       </c>
       <c r="L1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="N1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O1">
         <v>22</v>
       </c>
       <c r="P1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1636,28 +1660,28 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="L1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M1">
         <v>4</v>
@@ -1693,34 +1717,34 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J1">
         <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="L1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="M1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="N1">
         <v>5</v>
@@ -1756,22 +1780,22 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J1">
         <v>500</v>
@@ -1783,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="M1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N1" s="4">
         <v>4111111111111150</v>
@@ -1819,52 +1843,52 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G1">
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J1">
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="L1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="P1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="Q1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="R1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="S1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1894,37 +1918,37 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K1">
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="M1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="O1">
         <v>5</v>
@@ -1966,7 +1990,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -1999,22 +2023,22 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
         <v>93</v>
-      </c>
-      <c r="I1" t="s">
-        <v>98</v>
       </c>
       <c r="J1">
         <v>1</v>
@@ -2050,16 +2074,16 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G1">
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I1">
         <v>4111111111111110</v>
@@ -2071,22 +2095,22 @@
         <v>42379</v>
       </c>
       <c r="L1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" t="s">
         <v>101</v>
-      </c>
-      <c r="M1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" t="s">
-        <v>104</v>
-      </c>
-      <c r="P1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2120,7 +2144,7 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G1">
         <v>4111111111111110</v>
@@ -2129,7 +2153,7 @@
         <v>44166</v>
       </c>
       <c r="I1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J1" s="6">
         <v>10</v>
@@ -2193,13 +2217,13 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H1">
         <v>1</v>
@@ -2208,7 +2232,7 @@
         <v>36892</v>
       </c>
       <c r="J1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K1">
         <v>15</v>
@@ -2217,13 +2241,13 @@
         <v>36892</v>
       </c>
       <c r="M1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="P1" s="3">
         <v>36892</v>
@@ -2232,10 +2256,10 @@
         <v>20</v>
       </c>
       <c r="R1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="S1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="T1" s="3">
         <v>36892</v>
@@ -2244,10 +2268,10 @@
         <v>5</v>
       </c>
       <c r="V1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="W1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="X1" s="3">
         <v>36892</v>
@@ -2259,10 +2283,10 @@
         <v>14</v>
       </c>
       <c r="AA1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="AB1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="AC1" s="3">
         <v>36892</v>
@@ -2274,10 +2298,10 @@
         <v>3</v>
       </c>
       <c r="AF1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="AG1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AH1" s="3">
         <v>36892</v>
@@ -2325,22 +2349,22 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J1" s="3">
         <v>36893</v>
       </c>
       <c r="K1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L1" s="3">
         <v>36894</v>
@@ -2371,13 +2395,13 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G1" s="4">
         <v>411111111111111</v>
@@ -2392,31 +2416,31 @@
         <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L1">
         <v>42</v>
       </c>
       <c r="M1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="N1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="O1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="P1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="Q1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="R1" s="3">
         <v>37015</v>
       </c>
       <c r="S1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2444,16 +2468,16 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2483,40 +2507,40 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G1">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="M1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N1">
         <v>604</v>
       </c>
       <c r="O1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2549,31 +2573,31 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I1" s="3">
         <v>42690</v>
       </c>
       <c r="J1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="K1" t="s">
         <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="M1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2603,25 +2627,25 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E1">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K1">
         <v>1</v>
@@ -2630,7 +2654,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="N1">
         <v>1</v>
@@ -2639,13 +2663,13 @@
         <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="Q1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="R1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="S1">
         <v>1</v>
@@ -2703,7 +2727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2721,179 +2745,179 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1">
+        <v>345</v>
+      </c>
+      <c r="I1">
+        <v>345</v>
+      </c>
+      <c r="J1">
+        <v>3456</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R1" t="s">
+        <v>153</v>
+      </c>
+      <c r="S1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1">
+        <v>290211</v>
+      </c>
+      <c r="U1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" display="indianashu@gmail.com"/>
+    <hyperlink ref="O1" r:id="rId2" display="123, ad"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1">
+        <v>645</v>
+      </c>
+      <c r="I1">
+        <v>745</v>
+      </c>
+      <c r="J1">
+        <v>3678</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>159</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R1" t="s">
+        <v>153</v>
+      </c>
+      <c r="S1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1">
+        <v>902113</v>
+      </c>
+      <c r="U1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" display="indianashu@gmail.com"/>
+    <hyperlink ref="O1" r:id="rId2" display="123, ad"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
       </c>
       <c r="F1" t="s">
         <v>21</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
-      </c>
-      <c r="H1">
-        <v>91</v>
-      </c>
-      <c r="I1">
-        <v>98452</v>
-      </c>
-      <c r="J1">
-        <v>50449</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1">
-        <v>560035</v>
-      </c>
-      <c r="U1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K1" r:id="rId1"/>
-    <hyperlink ref="O1" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1">
-        <v>91</v>
-      </c>
-      <c r="I1">
-        <v>98452</v>
-      </c>
-      <c r="J1">
-        <v>50449</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1">
-        <v>560035</v>
-      </c>
-      <c r="U1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K1" r:id="rId1"/>
-    <hyperlink ref="O1" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2923,50 +2947,50 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new testcase for company hierarchy
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="622" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="622" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="161">
   <si>
     <t>test1234</t>
   </si>
@@ -2683,15 +2683,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -2714,7 +2714,10 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2810,7 +2813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
new code for discount and impersonate a customer
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -46,8 +46,9 @@
     <sheet name="Collections" sheetId="32" r:id="rId32"/>
     <sheet name="TearDown" sheetId="33" r:id="rId33"/>
     <sheet name="Discount" sheetId="34" r:id="rId34"/>
-    <sheet name="AddingAsset" sheetId="35" r:id="rId35"/>
-    <sheet name="Mediation" sheetId="36" r:id="rId36"/>
+    <sheet name="ImpersonateCust" sheetId="37" r:id="rId35"/>
+    <sheet name="AddingAsset" sheetId="35" r:id="rId36"/>
+    <sheet name="Mediation" sheetId="36" r:id="rId37"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="160">
   <si>
     <t>test1234</t>
   </si>
@@ -476,9 +477,6 @@
   </si>
   <si>
     <t>Please provide Discountable Item / Order and Discount on the Discount Line.</t>
-  </si>
-  <si>
-    <t>Plan Product</t>
   </si>
   <si>
     <t>Total = US$495.00</t>
@@ -1506,10 +1504,10 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
         <v>152</v>
-      </c>
-      <c r="G1" t="s">
-        <v>153</v>
       </c>
       <c r="H1" t="s">
         <v>75</v>
@@ -1524,7 +1522,7 @@
         <v>77</v>
       </c>
       <c r="L1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M1" s="5">
         <v>4111111111111150</v>
@@ -1602,16 +1600,16 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H1" t="s">
         <v>77</v>
       </c>
       <c r="I1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J1" s="5">
         <v>4111111111111150</v>
@@ -1620,25 +1618,25 @@
         <v>43862</v>
       </c>
       <c r="L1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" t="s">
         <v>155</v>
       </c>
-      <c r="M1" t="s">
-        <v>156</v>
-      </c>
       <c r="N1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O1">
         <v>23</v>
       </c>
       <c r="P1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R1" t="s">
         <v>158</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>154</v>
-      </c>
-      <c r="R1" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2504,7 +2502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2525,7 +2525,7 @@
         <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G1">
         <v>5</v>
@@ -2543,16 +2543,16 @@
         <v>137</v>
       </c>
       <c r="L1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N1">
         <v>604</v>
       </c>
       <c r="O1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2562,6 +2562,35 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -2588,7 +2617,7 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G1" t="s">
         <v>75</v>
@@ -2600,7 +2629,7 @@
         <v>42690</v>
       </c>
       <c r="J1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
@@ -2609,16 +2638,16 @@
         <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -2639,25 +2668,25 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E1">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
         <v>144</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>145</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>146</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>147</v>
-      </c>
-      <c r="J1" t="s">
-        <v>148</v>
       </c>
       <c r="K1">
         <v>1</v>
@@ -2666,7 +2695,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N1">
         <v>1</v>
@@ -2678,10 +2707,10 @@
         <v>36</v>
       </c>
       <c r="Q1" t="s">
+        <v>149</v>
+      </c>
+      <c r="R1" t="s">
         <v>150</v>
-      </c>
-      <c r="R1" t="s">
-        <v>151</v>
       </c>
       <c r="S1">
         <v>1</v>

</xml_diff>

<commit_message>
code change for testcase 12(12.1, 12.2)
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="27460" windowHeight="15860" tabRatio="622" firstSheet="20" activeTab="22"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="27460" windowHeight="15860" tabRatio="622" firstSheet="20" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -41,14 +41,15 @@
     <sheet name="AgentComProcess" sheetId="27" r:id="rId27"/>
     <sheet name="Reports" sheetId="28" r:id="rId28"/>
     <sheet name="MakePayment" sheetId="29" r:id="rId29"/>
-    <sheet name="BillingCreateOrders" sheetId="30" r:id="rId30"/>
-    <sheet name="Billing" sheetId="31" r:id="rId31"/>
-    <sheet name="Collections" sheetId="32" r:id="rId32"/>
-    <sheet name="TearDown" sheetId="33" r:id="rId33"/>
-    <sheet name="Discount" sheetId="34" r:id="rId34"/>
-    <sheet name="ImpersonateCust" sheetId="35" r:id="rId35"/>
-    <sheet name="AddingAsset" sheetId="36" r:id="rId36"/>
-    <sheet name="Mediation" sheetId="37" r:id="rId37"/>
+    <sheet name="BillCreateCustomers" sheetId="38" r:id="rId30"/>
+    <sheet name="BillCreateOrders" sheetId="30" r:id="rId31"/>
+    <sheet name="Billing" sheetId="31" r:id="rId32"/>
+    <sheet name="Collections" sheetId="32" r:id="rId33"/>
+    <sheet name="TearDown" sheetId="33" r:id="rId34"/>
+    <sheet name="Discount" sheetId="34" r:id="rId35"/>
+    <sheet name="ImpersonateCust" sheetId="35" r:id="rId36"/>
+    <sheet name="AddingAsset" sheetId="36" r:id="rId37"/>
+    <sheet name="Mediation" sheetId="37" r:id="rId38"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="159">
   <si>
     <t>test1234</t>
   </si>
@@ -534,6 +535,12 @@
   </si>
   <si>
     <t>Product Description</t>
+  </si>
+  <si>
+    <t>Billing1</t>
+  </si>
+  <si>
+    <t>Billing2</t>
   </si>
 </sst>
 </file>
@@ -588,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,6 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1773,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -2214,15 +2222,96 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="7">
+        <v>4111111111111150</v>
+      </c>
+      <c r="L1" s="11">
+        <v>43862</v>
+      </c>
+      <c r="M1" s="4">
+        <v>36892</v>
+      </c>
+      <c r="N1" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>36892</v>
+      </c>
+      <c r="U1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2233,105 +2322,84 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
+        <v>124</v>
+      </c>
+      <c r="G1" s="4">
+        <v>36892</v>
       </c>
       <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1" s="4">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="4">
         <v>36892</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
         <v>121</v>
       </c>
-      <c r="K1">
-        <v>15</v>
-      </c>
-      <c r="L1" s="4">
-        <v>36892</v>
-      </c>
-      <c r="M1" t="s">
-        <v>122</v>
-      </c>
       <c r="N1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="O1" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="P1" s="4">
         <v>36892</v>
       </c>
-      <c r="Q1">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>125</v>
+      <c r="Q1" s="4">
+        <v>36892</v>
+      </c>
+      <c r="R1">
+        <v>14</v>
       </c>
       <c r="S1" t="s">
-        <v>126</v>
-      </c>
-      <c r="T1" s="4">
+        <v>76</v>
+      </c>
+      <c r="T1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="4">
         <v>36892</v>
       </c>
-      <c r="U1">
-        <v>5</v>
-      </c>
-      <c r="V1" t="s">
-        <v>127</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="V1" s="4">
+        <v>36892</v>
+      </c>
+      <c r="W1">
+        <v>3</v>
+      </c>
+      <c r="X1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="4">
+      <c r="AA1" s="4">
         <v>36892</v>
       </c>
-      <c r="Y1" s="4">
+      <c r="AB1" s="4">
         <v>36892</v>
       </c>
-      <c r="Z1">
-        <v>14</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC1" s="4">
-        <v>36892</v>
-      </c>
-      <c r="AD1" s="4">
-        <v>36892</v>
-      </c>
-      <c r="AE1">
-        <v>3</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH1" s="4">
-        <v>36892</v>
-      </c>
-      <c r="AI1" s="4">
-        <v>36892</v>
-      </c>
-      <c r="AJ1">
-        <v>14</v>
-      </c>
-      <c r="AK1">
+      <c r="AC1">
+        <v>14</v>
+      </c>
+      <c r="AD1">
         <v>2</v>
       </c>
     </row>
@@ -2341,7 +2409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -2395,7 +2463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -2468,7 +2536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -2505,7 +2573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -2580,7 +2648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -2610,7 +2678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -2667,7 +2735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>

</xml_diff>

<commit_message>
code change for testcase-12(12.3,12.4,12.5)
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="27460" windowHeight="15860" tabRatio="622" firstSheet="20" activeTab="30"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="27460" windowHeight="15860" tabRatio="622" firstSheet="20" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -2305,7 +2305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2413,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
code change for testcases 16(16.1,16.2,16,3 and 16.4) and 18
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="26960" windowHeight="15900" tabRatio="622" firstSheet="27" activeTab="27"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28540" windowHeight="17320" tabRatio="622" firstSheet="23" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="156">
   <si>
     <t>test1234</t>
   </si>
@@ -369,21 +369,12 @@
     <t>The order has an error in the hierarchy field: Mandatory dependency not satisfied</t>
   </si>
   <si>
-    <t>Agent1</t>
-  </si>
-  <si>
-    <t>agent1@agent.com</t>
-  </si>
-  <si>
     <t>Master</t>
   </si>
   <si>
     <t>Invoice</t>
   </si>
   <si>
-    <t>Agent customer1</t>
-  </si>
-  <si>
     <t>Commissioned Product</t>
   </si>
   <si>
@@ -538,6 +529,9 @@
   </si>
   <si>
     <t>Test Mediation 2.0</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -592,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -606,6 +600,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1922,15 +1918,18 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+  <cols>
+    <col min="19" max="19" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1941,16 +1940,16 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" t="s">
         <v>102</v>
-      </c>
-      <c r="F1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" t="s">
-        <v>104</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
@@ -1959,19 +1958,19 @@
         <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K1">
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O1">
         <v>5</v>
@@ -1981,6 +1980,15 @@
       </c>
       <c r="Q1">
         <v>10</v>
+      </c>
+      <c r="R1">
+        <v>1</v>
+      </c>
+      <c r="S1" s="7">
+        <v>4111111111111150</v>
+      </c>
+      <c r="T1" s="12">
+        <v>43862</v>
       </c>
     </row>
   </sheetData>
@@ -2013,7 +2021,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -2029,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -2046,10 +2054,10 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F1" t="s">
         <v>76</v>
@@ -2058,10 +2066,10 @@
         <v>87</v>
       </c>
       <c r="H1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J1">
         <v>1</v>
@@ -2077,7 +2085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
@@ -2100,13 +2108,13 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G1">
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I1">
         <v>4111111111111110</v>
@@ -2118,19 +2126,19 @@
         <v>42379</v>
       </c>
       <c r="L1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" t="s">
         <v>115</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>116</v>
-      </c>
-      <c r="N1" t="s">
-        <v>117</v>
-      </c>
-      <c r="O1" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" t="s">
-        <v>119</v>
       </c>
       <c r="Q1" t="s">
         <v>60</v>
@@ -2245,7 +2253,7 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
         <v>76</v>
@@ -2257,7 +2265,7 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K1" s="7">
         <v>4111111111111150</v>
@@ -2269,10 +2277,10 @@
         <v>36892</v>
       </c>
       <c r="N1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="P1">
         <v>15</v>
@@ -2316,13 +2324,13 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G1" s="4">
         <v>36892</v>
@@ -2331,10 +2339,10 @@
         <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K1" s="4">
         <v>36892</v>
@@ -2343,10 +2351,10 @@
         <v>5</v>
       </c>
       <c r="M1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O1" t="s">
         <v>93</v>
@@ -2376,7 +2384,7 @@
         <v>3</v>
       </c>
       <c r="X1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Y1" t="s">
         <v>76</v>
@@ -2430,22 +2438,22 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J1" s="4">
         <v>36893</v>
       </c>
       <c r="K1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L1" s="4">
         <v>36894</v>
@@ -2478,13 +2486,13 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G1" s="7">
         <v>411111111111111</v>
@@ -2499,22 +2507,22 @@
         <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L1">
         <v>42</v>
       </c>
       <c r="M1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O1" t="s">
         <v>47</v>
       </c>
       <c r="P1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="Q1" t="s">
         <v>48</v>
@@ -2523,10 +2531,10 @@
         <v>37015</v>
       </c>
       <c r="S1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="T1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2557,13 +2565,13 @@
         <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2593,13 +2601,13 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G1">
         <v>5</v>
@@ -2608,13 +2616,13 @@
         <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L1" t="s">
         <v>59</v>
@@ -2626,16 +2634,16 @@
         <v>604</v>
       </c>
       <c r="O1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="P1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="Q1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="S1">
         <v>0</v>
@@ -2704,7 +2712,7 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G1" t="s">
         <v>76</v>
@@ -2755,25 +2763,25 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E1">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" t="s">
         <v>150</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>151</v>
-      </c>
-      <c r="H1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" t="s">
-        <v>154</v>
       </c>
       <c r="K1">
         <v>1</v>
@@ -2782,7 +2790,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="N1">
         <v>1</v>
@@ -2794,10 +2802,10 @@
         <v>36</v>
       </c>
       <c r="Q1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="S1">
         <v>1</v>

</xml_diff>

<commit_message>
Intellij Settings - Web Data Sanity - Standard Password
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="958" firstSheet="0" activeTab="33"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,490 +48,498 @@
     <sheet name="TearDown" sheetId="38" state="visible" r:id="rId39"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="160">
-  <si>
-    <t>test1234</t>
-  </si>
-  <si>
-    <t>ashutosh</t>
-  </si>
-  <si>
-    <t>sandhal</t>
-  </si>
-  <si>
-    <t>indianashu@gmail.com</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Indian Rupee</t>
-  </si>
-  <si>
-    <t>Colors World Ltd</t>
-  </si>
-  <si>
-    <t>123, ad</t>
-  </si>
-  <si>
-    <t>DC,213</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Successfully created Colors World Ltd. You can now login with the username test1234 after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Webdata@123</t>
-  </si>
-  <si>
-    <t>Web Data US</t>
-  </si>
-  <si>
-    <t>Marta</t>
-  </si>
-  <si>
-    <t>Kauffman</t>
-  </si>
-  <si>
-    <t>marta@weddatatech.in</t>
-  </si>
-  <si>
-    <t>United States Dollar</t>
-  </si>
-  <si>
-    <t>Web Data US Child</t>
-  </si>
-  <si>
-    <t>H-50</t>
-  </si>
-  <si>
-    <t>NewYork</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Successfully created Web Data US Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>S.Bright</t>
-  </si>
-  <si>
-    <t>kevin@weddatatech.in</t>
-  </si>
-  <si>
-    <t>Web Data US Reseller</t>
-  </si>
-  <si>
-    <t>Successfully created Web Data US Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t>Direct Customer</t>
-  </si>
-  <si>
-    <t>simple_invoice</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>Distributor Customer</t>
-  </si>
-  <si>
-    <t>Payment Card</t>
-  </si>
-  <si>
-    <t>Debit Card</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>Credit Card</t>
-  </si>
-  <si>
-    <t>Semi-monthly</t>
-  </si>
-  <si>
-    <t>Semi-Monthly</t>
-  </si>
-  <si>
-    <t>Payment Due</t>
-  </si>
-  <si>
-    <t>Grace Period</t>
-  </si>
-  <si>
-    <t>First Retry</t>
-  </si>
-  <si>
-    <t>Suspend</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.user.tasks.UserAgeingNotificationTask</t>
-  </si>
-  <si>
-    <t>'01/01/2001'</t>
-  </si>
-  <si>
-    <t>Child Entity Limited</t>
-  </si>
-  <si>
-    <t>Test category</t>
-  </si>
-  <si>
-    <t>New Test category</t>
-  </si>
-  <si>
-    <t>Asset Category1</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>In Use</t>
-  </si>
-  <si>
-    <t>Tax ID</t>
-  </si>
-  <si>
-    <t>Product Code1 Description</t>
-  </si>
-  <si>
-    <t>Product Code1</t>
-  </si>
-  <si>
-    <t>'10/11/2016'</t>
-  </si>
-  <si>
-    <t>'01/01/2002'</t>
-  </si>
-  <si>
-    <t>Test Code Description</t>
-  </si>
-  <si>
-    <t>Test Code</t>
-  </si>
-  <si>
-    <t>New Test Code Description</t>
-  </si>
-  <si>
-    <t>New Test Code</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.item.tasks.AssetUpdatedTask</t>
-  </si>
-  <si>
-    <t>SIM Cards</t>
-  </si>
-  <si>
-    <t>SIM</t>
-  </si>
-  <si>
-    <t>SIM-001</t>
-  </si>
-  <si>
-    <t>T-001</t>
-  </si>
-  <si>
-    <t>SIM-002</t>
-  </si>
-  <si>
-    <t>T-002</t>
-  </si>
-  <si>
-    <t>Copy Category</t>
-  </si>
-  <si>
-    <t>Test Copy Product Desc</t>
-  </si>
-  <si>
-    <t>Test Copy Product</t>
-  </si>
-  <si>
-    <t>Kevin S.Bright</t>
-  </si>
-  <si>
-    <t>Working as admin Web Data US Child X</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>james@weddatatech.in</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>abc.g@gmail.com</t>
-  </si>
-  <si>
-    <t>4111111111111152</t>
-  </si>
-  <si>
-    <t>02/2020</t>
-  </si>
-  <si>
-    <t>Lady Gaga</t>
-  </si>
-  <si>
-    <t>lgaga@billing.com</t>
-  </si>
-  <si>
-    <t>Jay Walker</t>
-  </si>
-  <si>
-    <t>jwalker@billing.com</t>
-  </si>
-  <si>
-    <t>user-24</t>
-  </si>
-  <si>
-    <t>Customer 23 receives invoices.</t>
-  </si>
-  <si>
-    <t>Test Discount1</t>
-  </si>
-  <si>
-    <t>AMOUNT_OR_PCT_BASED</t>
-  </si>
-  <si>
-    <t>Plan Product</t>
-  </si>
-  <si>
-    <t>Test Discount1 - Test Discount1:AMOUNT_OR_PCT_BASED</t>
-  </si>
-  <si>
-    <t>Please provide Discountable Item / Order and Discount on the Discount Line.</t>
-  </si>
-  <si>
-    <t>Total = US$495.00</t>
-  </si>
-  <si>
-    <t>Plan Category</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Customer A</t>
-  </si>
-  <si>
-    <t>pre paid</t>
-  </si>
-  <si>
-    <t>Asset Customer</t>
-  </si>
-  <si>
-    <t>Dependent Products</t>
-  </si>
-  <si>
-    <t>Installation Fee</t>
-  </si>
-  <si>
-    <t>D-01</t>
-  </si>
-  <si>
-    <t>Data Service</t>
-  </si>
-  <si>
-    <t>D-02</t>
-  </si>
-  <si>
-    <t>41 : Installation Fee</t>
-  </si>
-  <si>
-    <t>The order has an error in the hierarchy field: Mandatory dependency not satisfied</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
-  </si>
-  <si>
-    <t>asterisk.xml</t>
-  </si>
-  <si>
-    <t>csv</t>
-  </si>
-  <si>
-    <t>yyyyMMdd-HHmmss</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.mediation.task.TestMediationTask</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.mediation.task.SaveToFileMediationErrorHandler</t>
-  </si>
-  <si>
-    <t>MediationCustomer</t>
-  </si>
-  <si>
-    <t>Test Mediation 2.0</t>
-  </si>
-  <si>
-    <t>10/17/2016</t>
-  </si>
-  <si>
-    <t>Test Code1</t>
-  </si>
-  <si>
-    <t>Product Description</t>
-  </si>
-  <si>
-    <t>OneTime</t>
-  </si>
-  <si>
-    <t>post paid</t>
-  </si>
-  <si>
-    <t>Billing Customer1</t>
-  </si>
-  <si>
-    <t>Billing1</t>
-  </si>
-  <si>
-    <t>01/01/2001</t>
-  </si>
-  <si>
-    <t>Billing Customer2</t>
-  </si>
-  <si>
-    <t>Billing2</t>
-  </si>
-  <si>
-    <t>Billing Category</t>
-  </si>
-  <si>
-    <t>Billing Flat</t>
-  </si>
-  <si>
-    <t>Billing Graduated</t>
-  </si>
-  <si>
-    <t>One Time</t>
-  </si>
-  <si>
-    <t>italic</t>
-  </si>
-  <si>
-    <t>bold</t>
-  </si>
-  <si>
-    <t>01/16/2001</t>
-  </si>
-  <si>
-    <t>02/01/2001</t>
-  </si>
-  <si>
-    <t>03/01/2001</t>
-  </si>
-  <si>
-    <t>One time</t>
-  </si>
-  <si>
-    <t>Visa/master</t>
-  </si>
-  <si>
-    <t>rahul</t>
-  </si>
-  <si>
-    <t>4111111111111111</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>03/20/2001</t>
-  </si>
-  <si>
-    <t>03/25/2001</t>
-  </si>
-  <si>
-    <t>04/05/2001</t>
-  </si>
-  <si>
-    <t>US$10.00</t>
-  </si>
-  <si>
-    <t>TestCustomer3</t>
-  </si>
-  <si>
-    <t>10/01/2016</t>
-  </si>
-  <si>
-    <t>10/31/2016</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>View as HTML</t>
-  </si>
-  <si>
-    <t>Adobe PDF</t>
-  </si>
-  <si>
-    <t>Excel</t>
-  </si>
-  <si>
-    <t>Agent A</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Master</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>Customer B</t>
-  </si>
-  <si>
-    <t>Commissioned Product</t>
-  </si>
-  <si>
-    <t>Comm Product</t>
-  </si>
-  <si>
-    <t>C-01</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.user.partner.task.BasicPartnerCommissionTask</t>
-  </si>
-  <si>
-    <t>10/28/2016</t>
-  </si>
-  <si>
-    <t>US$1.00</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="161">
+  <si>
+    <t xml:space="preserve">test1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ashutosh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandhal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indianashu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indian Rupee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colors World Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123, ad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC,213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangalore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karnataka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created Colors World Ltd. You can now login with the username test1234 after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebData@101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data Sanity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kauffman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marta@weddatatech.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NewYork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created Web Data US Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kevin@weddatatech.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data Reseller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created Web Data US Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simple_invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributor Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debit Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semi-monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semi-Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment Due</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Retry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.user.tasks.UserAgeingNotificationTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/01/2001'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child Entity Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Test category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Category1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Code1 Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Code1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'10/11/2016'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/01/2002'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Code Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Test Code Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Test Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.item.tasks.AssetUpdatedTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM Cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copy Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Copy Product Desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Copy Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data US Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin S.Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working as admin Web Data US Child X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">james@weddatatech.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc.g@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4111111111111152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lady Gaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lgaga@billing.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jay Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jwalker@billing.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer 23 receives invoices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Discount1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMOUNT_OR_PCT_BASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Discount1 - Test Discount1:AMOUNT_OR_PCT_BASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please provide Discountable Item / Order and Discount on the Discount Line.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$495.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installation Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41 : Installation Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The order has an error in the hierarchy field: Mandatory dependency not satisfied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asterisk.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yyyyMMdd-HHmmss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.TestMediationTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.SaveToFileMediationErrorHandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MediationCustomer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Mediation 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/17/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Code1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OneTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Customer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Customer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Flat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Graduated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">italic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/16/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/01/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visa/master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rahul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4111111111111111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/20/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/25/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/05/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$10.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCustomer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/01/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/31/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View as HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adobe PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commissioned Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comm Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.user.partner.task.BasicPartnerCommissionTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/28/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$1.00</t>
   </si>
 </sst>
 </file>
@@ -539,13 +547,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0"/>
     <numFmt numFmtId="168" formatCode="MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -569,9 +577,91 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="12"/>
       <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -584,15 +674,57 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF222222"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -600,8 +732,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -625,20 +772,72 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -654,7 +853,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -671,29 +870,45 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -705,7 +920,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -721,7 +936,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -733,11 +948,11 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF222222"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF222222"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -750,13 +965,13 @@
   </sheetPr>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,7 +1034,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -834,13 +1049,13 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +1081,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -881,13 +1096,13 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,7 +1155,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -955,13 +1170,13 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +1189,7 @@
       <c r="C1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E1" s="0" t="n">
@@ -984,7 +1199,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -999,13 +1214,13 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,7 +1240,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1040,13 +1255,13 @@
   </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N41" activeCellId="0" sqref="N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,7 +1299,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1099,13 +1314,13 @@
   </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,7 +1348,7 @@
       <c r="H1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>57</v>
       </c>
       <c r="J1" s="0" t="s">
@@ -1145,7 +1360,7 @@
       <c r="L1" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="N1" s="0" t="s">
@@ -1179,7 +1394,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1194,13 +1409,13 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1452,7 @@
       <c r="K1" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>66</v>
       </c>
       <c r="M1" s="0" t="s">
@@ -1253,7 +1468,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1268,13 +1483,13 @@
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,7 +1514,7 @@
       <c r="G1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I1" s="0" t="s">
@@ -1318,7 +1533,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1333,13 +1548,13 @@
   </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,12 +1568,12 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G1" s="0" t="s">
@@ -1367,17 +1582,17 @@
       <c r="H1" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+      <c r="J1" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1392,13 +1607,13 @@
   </sheetPr>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,31 +1633,31 @@
         <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>39</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>80</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1666,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1466,20 +1681,20 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -1490,9 +1705,12 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="WebData@101"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1507,13 +1725,13 @@
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,43 +1751,43 @@
         <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="6" t="s">
         <v>82</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>39</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="L1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>23</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1578,7 +1796,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1593,13 +1811,13 @@
   </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,28 +1831,28 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>55</v>
@@ -1646,16 +1864,16 @@
         <v>604</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>0</v>
@@ -1664,7 +1882,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1679,13 +1897,13 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,13 +1917,13 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1720,13 +1938,13 @@
   </sheetPr>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,33 +1964,33 @@
         <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="J1" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="K1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="P1" s="0" t="n">
@@ -1785,7 +2003,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1800,13 +2018,13 @@
   </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q75" activeCellId="0" sqref="Q75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,15 +2044,15 @@
         <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="4" t="n">
         <v>42690</v>
       </c>
       <c r="J1" s="0" t="s">
@@ -1853,7 +2071,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1868,13 +2086,13 @@
   </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,58 +2106,58 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>98</v>
+      <c r="K1" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1954,13 +2172,13 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,25 +2192,25 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>1</v>
@@ -2001,7 +2219,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>1</v>
@@ -2013,10 +2231,10 @@
         <v>30</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>1</v>
@@ -2024,14 +2242,14 @@
       <c r="T1" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2046,13 +2264,13 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,22 +2284,22 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>55</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>4</v>
@@ -2090,10 +2308,10 @@
         <v>60</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>10</v>
@@ -2105,7 +2323,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2120,13 +2338,13 @@
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,31 +2358,31 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>55</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>55</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>500</v>
@@ -2176,19 +2394,19 @@
         <v>1</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q1" s="8" t="n">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="9" t="n">
         <v>4111111111111150</v>
       </c>
-      <c r="R1" s="9" t="n">
+      <c r="R1" s="10" t="n">
         <v>44166</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2203,13 +2421,13 @@
   </sheetPr>
   <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,10 +2447,10 @@
         <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
@@ -2241,45 +2459,45 @@
         <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>121</v>
+      <c r="L1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="N1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+      <c r="U1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2294,13 +2512,13 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,7 +2593,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2390,13 +2608,13 @@
   </sheetPr>
   <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AH1" activeCellId="0" sqref="AH1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,79 +2628,79 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>121</v>
+        <v>126</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>121</v>
+        <v>127</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="M1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>121</v>
+      <c r="Q1" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>14</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>121</v>
+        <v>97</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="W1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="X1" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>121</v>
+      <c r="AA1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="AC1" s="0" t="n">
         <v>14</v>
@@ -2494,7 +2712,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2509,13 +2727,13 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,104 +2746,104 @@
       <c r="C1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>121</v>
+      <c r="D1" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="J1" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="J1" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="K1" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>132</v>
+        <v>120</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="O1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="10" t="n">
+        <v>44166</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="9" t="n">
-        <v>44166</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>41</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>42</v>
@@ -2634,31 +2852,31 @@
         <v>42</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>43</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>140</v>
+      <c r="R1" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>45</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2673,13 +2891,13 @@
   </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2699,25 +2917,25 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>4111111111111110</v>
       </c>
-      <c r="H1" s="9" t="n">
+      <c r="H1" s="10" t="n">
         <v>44166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+        <v>76</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2732,13 +2950,13 @@
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2758,37 +2976,37 @@
         <v>30</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>143</v>
+      <c r="J1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>56</v>
@@ -2800,7 +3018,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2815,15 +3033,15 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="18" min="1" style="0" width="8.83333333333333"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.8333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="1" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2837,16 +3055,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="6" t="s">
         <v>150</v>
       </c>
+      <c r="E1" s="7" t="s">
+        <v>151</v>
+      </c>
       <c r="F1" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>15</v>
@@ -2855,19 +3073,19 @@
         <v>30</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -2881,11 +3099,11 @@
       <c r="R1" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="5" t="s">
+      <c r="S1" s="6" t="s">
         <v>80</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="U1" s="0" t="s">
         <v>39</v>
@@ -2897,7 +3115,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2912,13 +3130,13 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2932,7 +3150,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -2941,7 +3159,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2956,13 +3174,13 @@
   </sheetPr>
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2976,34 +3194,34 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+      <c r="K1" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3018,13 +3236,13 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3038,19 +3256,19 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>60</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3065,13 +3283,13 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3146,7 +3364,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3161,13 +3379,13 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,7 +3414,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3211,13 +3429,13 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3246,7 +3464,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3261,13 +3479,13 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3280,7 +3498,7 @@
       <c r="C1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -3293,7 +3511,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3308,13 +3526,13 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3333,7 +3551,7 @@
       <c r="E1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G1" s="0" t="n">
@@ -3343,7 +3561,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3358,13 +3576,13 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3377,7 +3595,7 @@
       <c r="C1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -3390,7 +3608,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Changes for the CustomerTest Package
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -766,7 +766,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="2" sqref="F1 L1 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -850,7 +850,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="2" sqref="F1 L1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -900,7 +900,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="2" sqref="F1 L1 M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -974,7 +974,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="2" sqref="F1 L1 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="2" sqref="F1 L1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="2" sqref="F1 L1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1118,7 +1118,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="2" sqref="F1 L1 S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1213,7 +1213,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="2" sqref="F1 L1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="F1 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1352,7 +1352,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="2" sqref="F1 L1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1410,8 +1410,8 @@
   </sheetPr>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1485,7 +1485,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1529,7 +1529,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="2" sqref="F1 L1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1615,7 +1615,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1657,10 +1657,10 @@
       <c r="K1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="5" t="s">
         <v>56</v>
       </c>
       <c r="N1" s="0" t="n">
@@ -1701,7 +1701,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="2" sqref="F1 L1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1742,7 +1742,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="2" sqref="F1 L1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1822,7 +1822,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="2" sqref="F1 L1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="2" sqref="F1 L1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1976,7 +1976,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="2" sqref="F1 L1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2068,7 +2068,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="2" sqref="F1 L1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2142,7 +2142,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2225,7 +2225,7 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="2" sqref="F1 L1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2316,7 +2316,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+      <selection pane="topLeft" activeCell="U2" activeCellId="2" sqref="F1 L1 U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2413,7 +2413,7 @@
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2532,7 +2532,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2606,7 +2606,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2695,7 +2695,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2754,7 +2754,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="2" sqref="F1 L1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2837,7 +2837,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="2" sqref="F1 L1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2934,7 +2934,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2978,7 +2978,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3040,7 +3040,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="F1 L1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3087,7 +3087,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="2" sqref="F1 L1 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3183,8 +3183,8 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="2" sqref="F1 L1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3234,7 +3234,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="2" sqref="F1 L1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3284,7 +3284,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+      <selection pane="topLeft" activeCell="I27" activeCellId="2" sqref="F1 L1 I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3331,7 +3331,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="2" sqref="F1 L1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3381,7 +3381,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="2" sqref="F1 L1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added the chnages for the OrderHierarchy Test
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -348,7 +348,7 @@
     <t>pre paid</t>
   </si>
   <si>
-    <t>Asset Customer</t>
+    <t>James4950</t>
   </si>
   <si>
     <t>Dependent Products</t>
@@ -1742,7 +1742,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1822,7 +1822,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1889,16 +1889,16 @@
   </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>13</v>
       </c>
@@ -3183,7 +3183,7 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes for the agent TearDown & MakePayment Test
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="24"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="162">
   <si>
     <t>test1234</t>
   </si>
@@ -348,7 +348,7 @@
     <t>pre paid</t>
   </si>
   <si>
-    <t>James4950</t>
+    <t>Asset Customer</t>
   </si>
   <si>
     <t>Dependent Products</t>
@@ -375,7 +375,7 @@
     <t>com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
   </si>
   <si>
-    <t>asterisk.xml</t>
+    <t>asterisk</t>
   </si>
   <si>
     <t>csv</t>
@@ -396,7 +396,7 @@
     <t>MediationCustomer</t>
   </si>
   <si>
-    <t>Test Mediation 2.0</t>
+    <t>Test Mediation2.0</t>
   </si>
   <si>
     <t>10/17/2016</t>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t>04/05/2001</t>
+  </si>
+  <si>
+    <t>James7998</t>
   </si>
   <si>
     <t>US$10.00</t>
@@ -1822,7 +1825,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1889,7 +1892,7 @@
   </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
@@ -1973,10 +1976,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1997,55 +2000,52 @@
       <c r="D1" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="0" t="n">
-        <v>1</v>
+      <c r="E1" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="J1" s="0" t="s">
         <v>111</v>
       </c>
+      <c r="J1" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="K1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L1" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="0" t="n">
-        <v>1</v>
+      <c r="M1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="R1" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="S1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T1" s="0" t="s">
+      <c r="R1" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="S1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2067,8 +2067,8 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2141,8 +2141,8 @@
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2695,7 +2695,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2720,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>4111111111111110</v>
@@ -2729,10 +2729,10 @@
         <v>44166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2753,8 +2753,8 @@
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2779,13 +2779,13 @@
         <v>31</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>80</v>
@@ -2794,22 +2794,22 @@
         <v>81</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>57</v>
@@ -2836,8 +2836,8 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2847,7 +2847,7 @@
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>13</v>
       </c>
@@ -2858,37 +2858,37 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -2934,7 +2934,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2953,7 +2953,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -2978,7 +2978,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2997,10 +2997,10 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>78</v>
@@ -3009,16 +3009,16 @@
         <v>97</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3039,8 +3039,8 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3059,7 +3059,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Fix the xpath of the billing
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="34"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -2412,6 +2412,199 @@
   </sheetPr>
   <dimension ref="A1:AD1"/>
   <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="R1" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="W1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC1" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD1" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -2432,199 +2625,6 @@
         <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="R1" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="W1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC1" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="AD1" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
         <v>123</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -2836,7 +2836,7 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes for the product and categorry controller
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="30"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,9 +52,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="162">
-  <si>
-    <t>test1234</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="159">
+  <si>
+    <t>admin</t>
   </si>
   <si>
     <t>ashutosh</t>
@@ -93,16 +93,10 @@
     <t>Successfully created Colors World Ltd. You can now login with the username test1234 after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Web Data</t>
-  </si>
-  <si>
-    <t>Web Data Sanity</t>
+    <t>Automated Sanity</t>
   </si>
   <si>
     <t>Marta</t>
@@ -117,7 +111,7 @@
     <t>United States Dollar</t>
   </si>
   <si>
-    <t>Web Data Child</t>
+    <t>Automated Sanity Child2</t>
   </si>
   <si>
     <t>H-50</t>
@@ -129,7 +123,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Successfully created Web Data US Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Successfully created Automated Sanity Child2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Kevin</t>
@@ -141,10 +135,10 @@
     <t>kevin@weddatatech.in</t>
   </si>
   <si>
-    <t>Web Data Reseller</t>
-  </si>
-  <si>
-    <t>Successfully created Web Data US Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Automated Sanity Reseller2</t>
+  </si>
+  <si>
+    <t>Successfully created Automated Sanity Reseller2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Direct Customer</t>
@@ -252,7 +246,7 @@
     <t>SIM Cards</t>
   </si>
   <si>
-    <t>SIM</t>
+    <t>SIM1</t>
   </si>
   <si>
     <t>SIM-001</t>
@@ -279,7 +273,7 @@
     <t>Kevin S.Bright</t>
   </si>
   <si>
-    <t>Working as admin Web Data Child X</t>
+    <t>Working as admin Automated Sanity Child2 X</t>
   </si>
   <si>
     <t>James</t>
@@ -348,7 +342,7 @@
     <t>pre paid</t>
   </si>
   <si>
-    <t>Asset Customer</t>
+    <t>Asset Customer1</t>
   </si>
   <si>
     <t>Dependent Products</t>
@@ -387,7 +381,7 @@
     <t>,</t>
   </si>
   <si>
-    <t>com.sapienter.jbilling.server.mediation.task.TestMediationTask</t>
+    <t>in.webdataconsulting.jbilling.server.mediation.tasks.WebDataTestAsteriskMediationTask</t>
   </si>
   <si>
     <t>com.sapienter.jbilling.server.mediation.task.SaveToFileMediationErrorHandler</t>
@@ -478,9 +472,6 @@
   </si>
   <si>
     <t>04/05/2001</t>
-  </si>
-  <si>
-    <t>James7998</t>
   </si>
   <si>
     <t>US$10.00</t>
@@ -769,7 +760,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -863,19 +854,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F1" s="0" t="n">
         <v>1</v>
@@ -913,40 +904,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>8</v>
@@ -977,7 +968,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -987,16 +978,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -1021,7 +1012,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1031,35 +1022,189 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>49</v>
       </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
+      <c r="E1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
@@ -1072,327 +1217,173 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="U1" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="V1" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>65</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="I1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="J1" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1424,46 +1415,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1488,7 +1479,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1498,16 +1489,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1532,7 +1523,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1542,58 +1533,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="M1" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="N1" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>23</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1628,58 +1619,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="L1" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>604</v>
       </c>
       <c r="O1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>95</v>
-      </c>
       <c r="R1" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>0</v>
@@ -1704,7 +1695,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1714,16 +1705,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1755,124 +1746,124 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q1" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I1" s="4" t="n">
         <v>42690</v>
       </c>
       <c r="J1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="L1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1892,7 +1883,7 @@
   </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
@@ -1903,117 +1894,117 @@
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="R1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="S1" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>111</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>2</v>
@@ -2022,31 +2013,31 @@
         <v>11</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2067,8 +2058,8 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2078,43 +2069,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="F1" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>4</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>10</v>
@@ -2152,141 +2143,141 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="K1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="9" t="n">
+        <v>4111111111111150</v>
+      </c>
+      <c r="R1" s="10" t="n">
+        <v>44166</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AN1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>118</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="N1" s="0" t="n">
-        <v>501</v>
-      </c>
-      <c r="O1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="9" t="n">
-        <v>4111111111111150</v>
-      </c>
-      <c r="R1" s="10" t="n">
-        <v>44166</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AN1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="0" t="s">
+      <c r="K1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="P1" s="0" t="n">
         <v>15</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="U1" s="4"/>
       <c r="Y1" s="4"/>
@@ -2315,8 +2306,8 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2326,25 +2317,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>345</v>
@@ -2356,37 +2347,37 @@
         <v>3456</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="P1" s="0" t="s">
         <v>8</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T1" s="0" t="n">
         <v>290211</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2423,88 +2414,88 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>14</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="W1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="X1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>122</v>
-      </c>
       <c r="AB1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AC1" s="0" t="n">
         <v>14</v>
@@ -2531,8 +2522,8 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2542,49 +2533,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="0" t="s">
+      <c r="J1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="K1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="M1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2616,83 +2607,142 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>137</v>
       </c>
       <c r="H1" s="10" t="n">
         <v>44166</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>41</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>42</v>
       </c>
       <c r="M1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="R1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="T1" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>4111111111111110</v>
+      </c>
+      <c r="H1" s="10" t="n">
+        <v>44166</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="Q1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -2705,117 +2755,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>4111111111111110</v>
-      </c>
-      <c r="H1" s="10" t="n">
-        <v>44166</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:R1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="M1" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="N1" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="Q1" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2849,46 +2840,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="H1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -2903,13 +2894,13 @@
         <v>1</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2944,16 +2935,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -2988,37 +2979,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>160</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3050,22 +3041,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3086,8 +3077,8 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3097,25 +3088,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>645</v>
@@ -3127,37 +3118,37 @@
         <v>3678</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="P1" s="0" t="s">
         <v>8</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T1" s="0" t="n">
         <v>902113</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3183,7 +3174,7 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -3194,22 +3185,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>32</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>33</v>
@@ -3226,7 +3267,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3244,169 +3332,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F1" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for the AIT field
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -96,7 +96,7 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Automated Sanity</t>
+    <t>Automated Sanity2</t>
   </si>
   <si>
     <t>Marta</t>
@@ -111,7 +111,7 @@
     <t>United States Dollar</t>
   </si>
   <si>
-    <t>Automated Sanity Child2</t>
+    <t>Automated Sanity2 Child2</t>
   </si>
   <si>
     <t>H-50</t>
@@ -123,7 +123,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Successfully created Automated Sanity Child2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Successfully created Automated Sanity2 Child2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Kevin</t>
@@ -135,10 +135,10 @@
     <t>kevin@weddatatech.in</t>
   </si>
   <si>
-    <t>Automated Sanity Reseller2</t>
-  </si>
-  <si>
-    <t>Successfully created Automated Sanity Reseller2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Automated Sanity2 Reseller2</t>
+  </si>
+  <si>
+    <t>Successfully created Automated Sanity2 Reseller2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Direct Customer</t>
@@ -273,7 +273,7 @@
     <t>Kevin S.Bright</t>
   </si>
   <si>
-    <t>Working as admin Automated Sanity Child2 X</t>
+    <t>Working as admin Automated Sanity2 Child2 X</t>
   </si>
   <si>
     <t>James</t>
@@ -760,7 +760,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -894,7 +894,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="1" sqref="C1 M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -968,7 +968,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="C1 S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1207,7 +1207,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="C1 L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1405,7 +1405,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1523,7 +1523,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C1 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1609,7 +1609,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1736,7 +1736,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="1" sqref="C1 H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1816,7 +1816,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="1" sqref="C1 M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1884,7 +1884,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1 N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="C1 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2059,7 +2059,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="1" sqref="C1 H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2133,7 +2133,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="C1 T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2216,7 +2216,7 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2307,7 +2307,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+      <selection pane="topLeft" activeCell="U1" activeCellId="1" sqref="C1 U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2404,7 +2404,7 @@
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="1" sqref="C1 M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2523,7 +2523,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="C1 K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2597,7 +2597,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2686,7 +2686,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="C1 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2745,7 +2745,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2828,7 +2828,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2925,7 +2925,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2969,7 +2969,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3031,7 +3031,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3078,7 +3078,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1 N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3175,7 +3175,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3275,7 +3275,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="C1 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3372,7 +3372,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added the Product for the Parent Company
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,7 +96,7 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Automated Sanity2</t>
+    <t>Web Data Sanity</t>
   </si>
   <si>
     <t>Marta</t>
@@ -111,7 +111,7 @@
     <t>United States Dollar</t>
   </si>
   <si>
-    <t>Automated Sanity2 Child2</t>
+    <t>Web Data Sanity Child2</t>
   </si>
   <si>
     <t>H-50</t>
@@ -123,7 +123,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Successfully created Automated Sanity2 Child2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Successfully created Web Data Sanity Child2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Kevin</t>
@@ -135,10 +135,10 @@
     <t>kevin@weddatatech.in</t>
   </si>
   <si>
-    <t>Automated Sanity2 Reseller2</t>
-  </si>
-  <si>
-    <t>Successfully created Automated Sanity2 Reseller2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Web Data Sanity Reseller2</t>
+  </si>
+  <si>
+    <t>Successfully created Web Data Sanity Reseller2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Direct Customer</t>
@@ -273,7 +273,7 @@
     <t>Kevin S.Bright</t>
   </si>
   <si>
-    <t>Working as admin Automated Sanity2 Child2 X</t>
+    <t>Working as admin Web Data Sanity Child2 X</t>
   </si>
   <si>
     <t>James</t>
@@ -760,7 +760,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -894,7 +894,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="1" sqref="C1 M1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -968,7 +968,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1111,8 +1111,8 @@
   </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="C1 S1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1207,7 +1207,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="1" sqref="C1 L1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1405,7 +1405,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1523,7 +1523,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C1 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1609,7 +1609,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1736,7 +1736,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="1" sqref="C1 H7"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1816,7 +1816,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="1" sqref="C1 M1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1884,7 +1884,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1 N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="C1 I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2059,7 +2059,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="1" sqref="C1 H17"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2133,7 +2133,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="C1 T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2216,7 +2216,7 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2307,7 +2307,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="1" sqref="C1 U1"/>
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2404,7 +2404,7 @@
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="1" sqref="C1 M1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2523,7 +2523,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="C1 K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2597,7 +2597,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2686,7 +2686,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="C1 I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2745,7 +2745,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2828,7 +2828,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2925,7 +2925,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2969,7 +2969,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3031,7 +3031,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3078,7 +3078,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1 N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3174,8 +3174,8 @@
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3275,7 +3275,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="C1 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3372,7 +3372,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add sleep in the Tests that have failed due to SleepTiming
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,7 +96,7 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Sanity Suite Test</t>
+    <t>Web Data 3</t>
   </si>
   <si>
     <t>Marta</t>
@@ -111,7 +111,7 @@
     <t>United States Dollar</t>
   </si>
   <si>
-    <t>Sanity Suite Test Child</t>
+    <t>Web Data 3 Child</t>
   </si>
   <si>
     <t>H-50</t>
@@ -123,7 +123,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Successfully created Sanity Suite Test Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Successfully created Web Data 3 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Kevin</t>
@@ -135,10 +135,10 @@
     <t>kevin@weddatatech.in</t>
   </si>
   <si>
-    <t>Sanity Suite Test Reseller2</t>
-  </si>
-  <si>
-    <t>Successfully created Sanity Suite Test Reseller2. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t>Web Data 3 Reseller</t>
+  </si>
+  <si>
+    <t>Successfully created Web Data 3 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t>Direct Customer</t>
@@ -273,7 +273,7 @@
     <t>Kevin S.Bright</t>
   </si>
   <si>
-    <t>Working as admin Sanity Suite Test Child X</t>
+    <t>Working as admin Web Data 3 Child X</t>
   </si>
   <si>
     <t>James</t>
@@ -894,7 +894,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1111,8 +1111,8 @@
   </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1969,8 +1969,8 @@
   </sheetPr>
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2037,7 +2037,7 @@
         <v>49</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2306,8 +2306,8 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3078,7 +3078,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fixes for the required sleep in the Sanity
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="25"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="160">
   <si>
     <t>admin</t>
   </si>
@@ -96,7 +96,7 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Web Data 3</t>
+    <t>Web Data 12</t>
   </si>
   <si>
     <t>Marta</t>
@@ -111,169 +111,172 @@
     <t>United States Dollar</t>
   </si>
   <si>
+    <t>Web Data 12 Child</t>
+  </si>
+  <si>
+    <t>H-50</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Successfully created Web Data 12 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>S.Bright</t>
+  </si>
+  <si>
+    <t>kevin@weddatatech.in</t>
+  </si>
+  <si>
+    <t>Web Data 12 Reseller</t>
+  </si>
+  <si>
+    <t>Successfully created Web Data 12 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+  </si>
+  <si>
+    <t>Direct Customer</t>
+  </si>
+  <si>
+    <t>main_simple_invoice</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Distributor</t>
+  </si>
+  <si>
+    <t>Distributor Customer</t>
+  </si>
+  <si>
+    <t>Payment Card</t>
+  </si>
+  <si>
+    <t>Debit Card</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>Semi-monthly</t>
+  </si>
+  <si>
+    <t>Semi-Monthly</t>
+  </si>
+  <si>
+    <t>Payment Due</t>
+  </si>
+  <si>
+    <t>Grace Period</t>
+  </si>
+  <si>
+    <t>First Retry</t>
+  </si>
+  <si>
+    <t>Suspend</t>
+  </si>
+  <si>
+    <t>com.sapienter.jbilling.server.user.tasks.UserAgeingNotificationTask</t>
+  </si>
+  <si>
+    <t>'01/01/2001'</t>
+  </si>
+  <si>
+    <t>Child Entity Limited</t>
+  </si>
+  <si>
+    <t>Test category</t>
+  </si>
+  <si>
+    <t>New Test category</t>
+  </si>
+  <si>
+    <t>Asset Category1</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>In Use</t>
+  </si>
+  <si>
+    <t>Tax ID</t>
+  </si>
+  <si>
+    <t>Product Code1 Description</t>
+  </si>
+  <si>
+    <t>Product Code1</t>
+  </si>
+  <si>
+    <t>'10/11/2016'</t>
+  </si>
+  <si>
+    <t>'01/01/2002'</t>
+  </si>
+  <si>
+    <t>Test Code Description</t>
+  </si>
+  <si>
+    <t>Test Code</t>
+  </si>
+  <si>
+    <t>New Test Code Description</t>
+  </si>
+  <si>
+    <t>New Test Code</t>
+  </si>
+  <si>
+    <t>com.sapienter.jbilling.server.item.tasks.AssetUpdatedTask</t>
+  </si>
+  <si>
+    <t>SIM Cards</t>
+  </si>
+  <si>
+    <t>SIM1</t>
+  </si>
+  <si>
+    <t>SIM-001</t>
+  </si>
+  <si>
+    <t>T-001</t>
+  </si>
+  <si>
+    <t>SIM-002</t>
+  </si>
+  <si>
+    <t>T-002</t>
+  </si>
+  <si>
+    <t>Copy Category</t>
+  </si>
+  <si>
+    <t>Test Copy Product Desc</t>
+  </si>
+  <si>
+    <t>Test Copy Product</t>
+  </si>
+  <si>
     <t>Web Data 3 Child</t>
   </si>
   <si>
-    <t>H-50</t>
-  </si>
-  <si>
-    <t>NewYork</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Successfully created Web Data 3 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>S.Bright</t>
-  </si>
-  <si>
-    <t>kevin@weddatatech.in</t>
-  </si>
-  <si>
-    <t>Web Data 3 Reseller</t>
-  </si>
-  <si>
-    <t>Successfully created Web Data 3 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
-  </si>
-  <si>
-    <t>Direct Customer</t>
-  </si>
-  <si>
-    <t>main_new_invoice_design</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>Distributor Customer</t>
-  </si>
-  <si>
-    <t>Payment Card</t>
-  </si>
-  <si>
-    <t>Debit Card</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>Credit Card</t>
-  </si>
-  <si>
-    <t>Semi-monthly</t>
-  </si>
-  <si>
-    <t>Semi-Monthly</t>
-  </si>
-  <si>
-    <t>Payment Due</t>
-  </si>
-  <si>
-    <t>Grace Period</t>
-  </si>
-  <si>
-    <t>First Retry</t>
-  </si>
-  <si>
-    <t>Suspend</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.user.tasks.UserAgeingNotificationTask</t>
-  </si>
-  <si>
-    <t>'01/01/2001'</t>
-  </si>
-  <si>
-    <t>Child Entity Limited</t>
-  </si>
-  <si>
-    <t>Test category</t>
-  </si>
-  <si>
-    <t>New Test category</t>
-  </si>
-  <si>
-    <t>Asset Category1</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>In Use</t>
-  </si>
-  <si>
-    <t>Tax ID</t>
-  </si>
-  <si>
-    <t>Product Code1 Description</t>
-  </si>
-  <si>
-    <t>Product Code1</t>
-  </si>
-  <si>
-    <t>'10/11/2016'</t>
-  </si>
-  <si>
-    <t>'01/01/2002'</t>
-  </si>
-  <si>
-    <t>Test Code Description</t>
-  </si>
-  <si>
-    <t>Test Code</t>
-  </si>
-  <si>
-    <t>New Test Code Description</t>
-  </si>
-  <si>
-    <t>New Test Code</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.item.tasks.AssetUpdatedTask</t>
-  </si>
-  <si>
-    <t>SIM Cards</t>
-  </si>
-  <si>
-    <t>SIM1</t>
-  </si>
-  <si>
-    <t>SIM-001</t>
-  </si>
-  <si>
-    <t>T-001</t>
-  </si>
-  <si>
-    <t>SIM-002</t>
-  </si>
-  <si>
-    <t>T-002</t>
-  </si>
-  <si>
-    <t>Copy Category</t>
-  </si>
-  <si>
-    <t>Test Copy Product Desc</t>
-  </si>
-  <si>
-    <t>Test Copy Product</t>
-  </si>
-  <si>
     <t>Kevin S.Bright</t>
   </si>
   <si>
-    <t>Working as admin Web Data 3 Child X</t>
+    <t>Working as admin Web Data 12 Child X</t>
   </si>
   <si>
     <t>James</t>
@@ -1281,7 +1284,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1346,7 +1349,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1365,7 +1368,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>50</v>
@@ -1380,10 +1383,10 @@
         <v>67</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1430,31 +1433,31 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>38</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1548,43 +1551,43 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>38</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="L1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>23</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1628,28 +1631,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>54</v>
@@ -1661,16 +1664,16 @@
         <v>604</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>0</v>
@@ -1714,7 +1717,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1761,25 +1764,25 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>38</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>57</v>
@@ -1841,13 +1844,13 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="I1" s="4" t="n">
         <v>42690</v>
@@ -1884,7 +1887,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1903,52 +1906,52 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1969,7 +1972,7 @@
   </sheetPr>
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
@@ -1989,22 +1992,22 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>2</v>
@@ -2013,7 +2016,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>2</v>
@@ -2025,10 +2028,10 @@
         <v>29</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>12</v>
@@ -2078,22 +2081,22 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>54</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>4</v>
@@ -2102,10 +2105,10 @@
         <v>59</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>10</v>
@@ -2152,31 +2155,31 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>500</v>
@@ -2188,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q1" s="9" t="n">
         <v>4111111111111150</v>
@@ -2241,10 +2244,10 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
@@ -2253,28 +2256,28 @@
         <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P1" s="0" t="n">
         <v>15</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>38</v>
@@ -2307,7 +2310,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2423,79 +2426,79 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="M1" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="Q1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>14</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="W1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="X1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="Y1" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="AA1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AC1" s="0" t="n">
         <v>14</v>
@@ -2542,40 +2545,40 @@
         <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2616,28 +2619,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H1" s="10" t="n">
         <v>44166</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>41</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>42</v>
@@ -2646,25 +2649,25 @@
         <v>41</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>42</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>43</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2711,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>4111111111111110</v>
@@ -2720,10 +2723,10 @@
         <v>44166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2770,37 +2773,37 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>55</v>
@@ -2849,16 +2852,16 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>14</v>
@@ -2867,19 +2870,19 @@
         <v>29</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -2894,10 +2897,10 @@
         <v>1</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="U1" s="0" t="s">
         <v>38</v>
@@ -2944,7 +2947,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -2988,28 +2991,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3050,13 +3053,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>59</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3077,8 +3080,8 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3175,7 +3178,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added select currency code in every Customer and Product Creation Page
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="160">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -768,7 +768,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -852,7 +852,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,7 +902,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -976,7 +976,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1061,7 +1061,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="V1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1119,8 +1119,8 @@
   </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="V1 O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="V1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1289,7 +1289,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="V1 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1354,7 +1354,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="V1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1410,10 +1410,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="V1 O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1421,7 +1421,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1463,6 +1463,9 @@
       </c>
       <c r="N1" s="6" t="s">
         <v>80</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1486,8 +1489,8 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="V1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1528,10 +1531,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P7" activeCellId="1" sqref="V1 P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1539,7 +1542,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1593,6 +1596,9 @@
       </c>
       <c r="R1" s="0" t="s">
         <v>86</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1623,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1703,7 +1709,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1741,18 +1747,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <selection pane="topLeft" activeCell="R1" activeCellId="1" sqref="V1 R1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="1" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1804,6 +1812,9 @@
       <c r="Q1" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="R1" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1821,18 +1832,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="V1 N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1872,6 +1885,9 @@
       <c r="M1" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="N1" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1889,10 +1905,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="V1 T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1900,7 +1916,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1958,6 +1974,9 @@
       <c r="S1" s="0" t="s">
         <v>99</v>
       </c>
+      <c r="T1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1978,7 +1997,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="V1 T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2064,10 +2083,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="V1 P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2121,6 +2140,9 @@
       <c r="O1" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2141,7 +2163,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="V1 T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2224,15 +2246,17 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="V1 S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="1" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2286,6 +2310,9 @@
       </c>
       <c r="R1" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="U1" s="4"/>
       <c r="Y1" s="4"/>
@@ -2315,7 +2342,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="V1 N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2409,18 +2436,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+  <dimension ref="A1:AE1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE1" activeCellId="1" sqref="V1 AE1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="1" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="32" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2511,6 +2540,9 @@
       <c r="AD1" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="AE1" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2531,7 +2563,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="V1 K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2605,7 +2637,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2694,7 +2726,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="V1 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2750,10 +2782,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="V1 S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2816,6 +2848,9 @@
       <c r="R1" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2833,10 +2868,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2846,7 +2881,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2909,6 +2944,9 @@
       </c>
       <c r="U1" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2933,7 +2971,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2977,7 +3015,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="V1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3039,7 +3077,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3086,7 +3124,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="V1 N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3180,10 +3218,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="V1 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3213,6 +3251,9 @@
       <c r="G1" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3233,7 +3274,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3283,7 +3324,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3330,7 +3371,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3380,7 +3421,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="V1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added One Class to avoid the Stale Element Reference Exception
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="34"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="159">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Simple Biliing Sanity</t>
+    <t xml:space="preserve">Web Data 37</t>
   </si>
   <si>
     <t xml:space="preserve">Marta</t>
@@ -116,7 +116,7 @@
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Simple Biliing Sanity Child</t>
+    <t xml:space="preserve">Web Data 37 Child</t>
   </si>
   <si>
     <t xml:space="preserve">H-50</t>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">Successfully created Simple Biliing Sanity Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Successfully created Web Data 37 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Kevin</t>
@@ -140,10 +140,10 @@
     <t xml:space="preserve">kevin@weddatatech.in</t>
   </si>
   <si>
-    <t xml:space="preserve">Simple Biliing Sanity Reseller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Successfully created Simple Biliing Sanity Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Web Data 37 Reseller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created Web Data 37 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Direct Customer</t>
@@ -275,13 +275,10 @@
     <t xml:space="preserve">Test Copy Product</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 3 Child</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kevin S.Bright</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Simple Biliing Sanity Child X</t>
+    <t xml:space="preserve">Working as admin Web Data 37 Child X</t>
   </si>
   <si>
     <t xml:space="preserve">James</t>
@@ -768,7 +765,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -852,7 +849,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -901,8 +898,8 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -976,7 +973,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1020,7 +1017,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1061,7 +1058,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="V1 J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1120,7 +1117,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="V1 O1"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,7 +1212,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="V1 J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1289,7 +1286,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="V1 I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1354,7 +1351,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="V1 J1"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1373,7 +1370,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>50</v>
@@ -1388,11 +1385,11 @@
         <v>67</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>74</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1413,7 +1410,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="V1 O1"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1438,31 +1435,31 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>38</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>18</v>
@@ -1490,7 +1487,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="V1 E1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1534,7 +1531,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P7" activeCellId="1" sqref="V1 P7"/>
+      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1559,43 +1556,43 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>38</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>81</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>23</v>
       </c>
       <c r="P1" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>18</v>
@@ -1623,7 +1620,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1642,28 +1639,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>54</v>
@@ -1675,16 +1672,16 @@
         <v>604</v>
       </c>
       <c r="O1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="Q1" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="R1" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>0</v>
@@ -1709,7 +1706,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1728,7 +1725,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1750,7 +1747,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="1" sqref="V1 R1"/>
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1777,25 +1774,25 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>38</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>57</v>
@@ -1835,7 +1832,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="V1 N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1862,13 +1859,13 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I1" s="4" t="n">
         <v>42690</v>
@@ -1908,7 +1905,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="V1 T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1927,52 +1924,52 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>102</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>18</v>
@@ -1997,7 +1994,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="V1 T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2016,22 +2013,22 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>2</v>
@@ -2040,7 +2037,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>2</v>
@@ -2052,10 +2049,10 @@
         <v>29</v>
       </c>
       <c r="P1" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>12</v>
@@ -2086,7 +2083,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="V1 P1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2105,22 +2102,22 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>54</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>4</v>
@@ -2129,10 +2126,10 @@
         <v>59</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>10</v>
@@ -2163,7 +2160,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="V1 T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2182,31 +2179,31 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>118</v>
       </c>
       <c r="K1" s="0" t="s">
         <v>54</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>500</v>
@@ -2218,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="9" t="n">
         <v>4111111111111150</v>
@@ -2246,7 +2243,7 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="V1 S1"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2273,10 +2270,10 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
@@ -2285,28 +2282,28 @@
         <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>123</v>
       </c>
       <c r="P1" s="0" t="n">
         <v>15</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>38</v>
@@ -2342,7 +2339,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="V1 N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2439,7 +2436,7 @@
   <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE1" activeCellId="1" sqref="V1 AE1"/>
+      <selection pane="topLeft" activeCell="AE1" activeCellId="0" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2460,79 +2457,79 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>125</v>
-      </c>
       <c r="F1" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>14</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC1" s="0" t="n">
         <v>14</v>
@@ -2563,7 +2560,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="V1 K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2582,102 +2579,102 @@
         <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="O1" s="8" t="s">
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>133</v>
       </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1 A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="H1" s="10" t="n">
         <v>44166</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>41</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>42</v>
@@ -2686,25 +2683,25 @@
         <v>41</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>42</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>43</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>44</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2726,7 +2723,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="V1 I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2751,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>4111111111111110</v>
@@ -2760,10 +2757,10 @@
         <v>44166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2785,7 +2782,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="V1 S1"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2810,37 +2807,37 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>55</v>
@@ -2870,7 +2867,7 @@
   </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
     </sheetView>
   </sheetViews>
@@ -2892,16 +2889,16 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>14</v>
@@ -2910,19 +2907,19 @@
         <v>29</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>156</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -2937,10 +2934,10 @@
         <v>1</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="U1" s="0" t="s">
         <v>38</v>
@@ -2971,7 +2968,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2990,7 +2987,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -3015,7 +3012,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="V1 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3034,28 +3031,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3077,7 +3074,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="V1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3096,13 +3093,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>59</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3124,7 +3121,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="V1 N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3221,7 +3218,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="V1 H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3274,7 +3271,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3324,7 +3321,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3371,7 +3368,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="V1 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3421,7 +3418,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="V1 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added PDF Notification Invoice Plugin Page
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,6 +46,7 @@
     <sheet name="AgentPlugin" sheetId="36" state="visible" r:id="rId37"/>
     <sheet name="AgentComProcess" sheetId="37" state="visible" r:id="rId38"/>
     <sheet name="TearDown" sheetId="38" state="visible" r:id="rId39"/>
+    <sheet name="configInvoicePlugin" sheetId="39" state="visible" r:id="rId40"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="161">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -101,7 +102,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 37</t>
+    <t xml:space="preserve">Web Data 38</t>
   </si>
   <si>
     <t xml:space="preserve">Marta</t>
@@ -116,7 +117,7 @@
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 37 Child</t>
+    <t xml:space="preserve">Web Data 38 Child</t>
   </si>
   <si>
     <t xml:space="preserve">H-50</t>
@@ -128,7 +129,7 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">Successfully created Web Data 37 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Successfully created Web Data 38 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Kevin</t>
@@ -140,24 +141,27 @@
     <t xml:space="preserve">kevin@weddatatech.in</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 37 Reseller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Successfully created Web Data 37 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Web Data 38 Reseller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created Web Data 38 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Direct Customer</t>
   </si>
   <si>
+    <t xml:space="preserve">main_mastercard_invoice_design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributor</t>
+  </si>
+  <si>
     <t xml:space="preserve">main_simple_invoice</t>
   </si>
   <si>
-    <t xml:space="preserve">Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distributor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Distributor Customer</t>
   </si>
   <si>
@@ -278,7 +282,7 @@
     <t xml:space="preserve">Kevin S.Bright</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Web Data 37 Child X</t>
+    <t xml:space="preserve">Working as admin Web Data 38 Child X</t>
   </si>
   <si>
     <t xml:space="preserve">James</t>
@@ -534,18 +538,22 @@
   </si>
   <si>
     <t xml:space="preserve">US$1.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sql_query</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0"/>
     <numFmt numFmtId="168" formatCode="MM/YY"/>
+    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -639,7 +647,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -681,6 +689,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -868,10 +880,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="0" t="n">
         <v>1</v>
@@ -898,7 +910,7 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -918,31 +930,31 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>8</v>
@@ -992,7 +1004,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -1036,7 +1048,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1077,25 +1089,25 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1136,13 +1148,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>29</v>
@@ -1151,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>14</v>
@@ -1163,7 +1175,7 @@
         <v>500</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>14</v>
@@ -1175,10 +1187,10 @@
         <v>50</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>14</v>
@@ -1187,10 +1199,10 @@
         <v>10</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1231,19 +1243,19 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>14</v>
@@ -1255,16 +1267,16 @@
         <v>2</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1305,19 +1317,19 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>14</v>
@@ -1351,7 +1363,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1373,22 +1385,22 @@
         <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1435,31 +1447,31 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>18</v>
@@ -1556,43 +1568,43 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="L1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>23</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>18</v>
@@ -1639,49 +1651,49 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>604</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>0</v>
@@ -1725,7 +1737,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1774,34 +1786,34 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P1" s="0" t="n">
         <v>2</v>
@@ -1859,28 +1871,28 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="I1" s="4" t="n">
         <v>42690</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>18</v>
@@ -1924,52 +1936,52 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>18</v>
@@ -2013,22 +2025,22 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>2</v>
@@ -2037,7 +2049,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>2</v>
@@ -2049,19 +2061,19 @@
         <v>29</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2102,34 +2114,34 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>4</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>10</v>
@@ -2159,8 +2171,8 @@
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2179,31 +2191,31 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>115</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>500</v>
@@ -2215,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q1" s="9" t="n">
         <v>4111111111111150</v>
@@ -2270,10 +2282,10 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
@@ -2282,31 +2294,31 @@
         <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P1" s="0" t="n">
         <v>15</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S1" s="8" t="s">
         <v>18</v>
@@ -2457,79 +2469,79 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="M1" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="Q1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>14</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="W1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="X1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="Y1" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="AA1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AC1" s="0" t="n">
         <v>14</v>
@@ -2579,40 +2591,40 @@
         <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2653,55 +2665,55 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H1" s="10" t="n">
         <v>44166</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>41</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>42</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2748,7 +2760,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>4111111111111110</v>
@@ -2757,10 +2769,10 @@
         <v>44166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2807,43 +2819,43 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>18</v>
@@ -2889,16 +2901,16 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>14</v>
@@ -2907,19 +2919,19 @@
         <v>29</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -2934,13 +2946,13 @@
         <v>1</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V1" s="0" t="s">
         <v>18</v>
@@ -2987,7 +2999,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -3031,28 +3043,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3074,7 +3086,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3093,22 +3105,67 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.36"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3218,7 +3275,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3296,10 +3353,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3340,13 +3397,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3387,13 +3444,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
@@ -3437,10 +3494,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Added Filter for Customer in the Sanity Plan
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -102,7 +102,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 38</t>
+    <t xml:space="preserve">Web Data 49</t>
   </si>
   <si>
     <t xml:space="preserve">Marta</t>
@@ -117,7 +117,7 @@
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 38 Child</t>
+    <t xml:space="preserve">Web Data 49 Child</t>
   </si>
   <si>
     <t xml:space="preserve">H-50</t>
@@ -129,7 +129,7 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">Successfully created Web Data 38 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Successfully created Web Data 49 Child. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Kevin</t>
@@ -141,10 +141,10 @@
     <t xml:space="preserve">kevin@weddatatech.in</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 38 Reseller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Successfully created Web Data 38 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
+    <t xml:space="preserve">Web Data 49 Reseller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully created Web Data 49 Reseller. You can now login with the username admin after your password is set. Password reset link is sent to your email.</t>
   </si>
   <si>
     <t xml:space="preserve">Direct Customer</t>
@@ -282,7 +282,7 @@
     <t xml:space="preserve">Kevin S.Bright</t>
   </si>
   <si>
-    <t xml:space="preserve">Working as admin Web Data 38 Child X</t>
+    <t xml:space="preserve">Working as admin Web Data 49 Child X</t>
   </si>
   <si>
     <t xml:space="preserve">James</t>
@@ -777,7 +777,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -911,7 +911,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="1" sqref="C1 G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -985,7 +985,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1070,7 +1070,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="C1 O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1224,7 +1224,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1298,7 +1298,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="C1 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1363,7 +1363,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1422,7 +1422,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="1" sqref="C1 O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
+      <selection pane="topLeft" activeCell="P7" activeCellId="1" sqref="C1 P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1632,7 +1632,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1718,7 +1718,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1759,7 +1759,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="topLeft" activeCell="R1" activeCellId="1" sqref="C1 R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1844,7 +1844,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1 N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="C1 T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2006,7 +2006,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="1" sqref="C1 T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2095,7 +2095,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="C1 P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2172,7 +2172,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2255,7 +2255,7 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="C1 S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2351,7 +2351,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1 N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2448,7 +2448,7 @@
   <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE1" activeCellId="0" sqref="AE1"/>
+      <selection pane="topLeft" activeCell="AE1" activeCellId="1" sqref="C1 AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2572,7 +2572,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="C1 K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2646,7 +2646,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2735,7 +2735,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="C1 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2794,7 +2794,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="1" sqref="C1 S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2880,7 +2880,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="topLeft" activeCell="V1" activeCellId="1" sqref="C1 V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2980,7 +2980,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3024,7 +3024,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3086,7 +3086,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3178,7 +3178,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="1" sqref="C1 N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3275,7 +3275,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3475,7 +3475,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Changed the name of the invoice design in account type sheet
</commit_message>
<xml_diff>
--- a/Webdata_TestData.xlsx
+++ b/Webdata_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="SignupData" sheetId="1" state="visible" r:id="rId2"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="160">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">Distributor</t>
   </si>
   <si>
-    <t xml:space="preserve">main_simple_invoice</t>
-  </si>
-  <si>
     <t xml:space="preserve">Distributor Customer</t>
   </si>
   <si>
@@ -234,121 +231,121 @@
     <t xml:space="preserve">'10/11/2016'</t>
   </si>
   <si>
+    <t xml:space="preserve">Test Code Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Test Code Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Test Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.item.tasks.AssetUpdatedTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM Cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copy Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Copy Product Desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Copy Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin S.Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working as admin Web Data 1 Child X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">james@weddatatech.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc.g@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4111111111111152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lady Gaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lgaga@billing.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jay Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jwalker@billing.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer 23 receives invoices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Discount1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMOUNT_OR_PCT_BASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Discount1 - Test Discount1:AMOUNT_OR_PCT_BASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please provide Discountable Item / Order and Discount on the Discount Line.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$495.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
     <t xml:space="preserve">'01/01/2002'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Code Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Test Code Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Test Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.sapienter.jbilling.server.item.tasks.AssetUpdatedTask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM Cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copy Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Copy Product Desc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Copy Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin S.Bright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Working as admin Web Data 1 Child X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">james@weddatatech.in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abc.g@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4111111111111152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lady Gaga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lgaga@billing.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jay Walker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jwalker@billing.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer 23 receives invoices.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Discount1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMOUNT_OR_PCT_BASED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Discount1 - Test Discount1:AMOUNT_OR_PCT_BASED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please provide Discountable Item / Order and Discount on the Discount Line.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total = US$495.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pre paid</t>
   </si>
   <si>
     <t xml:space="preserve">Asset Customer1</t>
@@ -880,10 +877,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F1" s="0" t="n">
         <v>1</v>
@@ -930,31 +927,31 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>8</v>
@@ -1004,7 +1001,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -1048,7 +1045,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1089,47 +1086,216 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="E1" s="0" t="s">
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>50</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
+        <v>18</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1148,80 +1314,50 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="L1" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="U1" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="V1" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
@@ -1243,164 +1379,25 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>51</v>
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>64</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="I1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="J1" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1447,31 +1444,31 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>18</v>
@@ -1568,43 +1565,43 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="M1" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="N1" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>81</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>23</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>18</v>
@@ -1651,49 +1648,49 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>91</v>
-      </c>
       <c r="L1" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N1" s="0" t="n">
         <v>604</v>
       </c>
       <c r="O1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="P1" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="R1" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S1" s="0" t="n">
         <v>0</v>
@@ -1737,7 +1734,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1786,34 +1783,34 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="0" t="s">
+      <c r="N1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="P1" s="0" t="n">
         <v>2</v>
@@ -1871,28 +1868,28 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I1" s="4" t="n">
         <v>42690</v>
       </c>
       <c r="J1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="L1" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>18</v>
@@ -1936,52 +1933,52 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>102</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>18</v>
@@ -2025,22 +2022,22 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>2</v>
@@ -2049,7 +2046,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M1" s="0" t="n">
         <v>2</v>
@@ -2061,19 +2058,19 @@
         <v>29</v>
       </c>
       <c r="P1" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2114,109 +2111,109 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="F1" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>4</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="N1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="O1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:R1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>116</v>
-      </c>
       <c r="M1" s="0" t="n">
         <v>500</v>
       </c>
@@ -2227,7 +2224,7 @@
         <v>1</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="9" t="n">
         <v>4111111111111150</v>
@@ -2282,10 +2279,10 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>1</v>
@@ -2294,31 +2291,31 @@
         <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>123</v>
       </c>
       <c r="P1" s="0" t="n">
         <v>15</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S1" s="8" t="s">
         <v>18</v>
@@ -2469,79 +2466,79 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>125</v>
-      </c>
       <c r="F1" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>20</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>5</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R1" s="0" t="n">
         <v>14</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W1" s="0" t="n">
         <v>3</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC1" s="0" t="n">
         <v>14</v>
@@ -2591,40 +2588,40 @@
         <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2665,55 +2662,55 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="H1" s="10" t="n">
         <v>44166</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>41</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>42</v>
       </c>
       <c r="M1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="R1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="T1" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2760,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>4111111111111110</v>
@@ -2769,10 +2766,10 @@
         <v>44166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2819,43 +2816,43 @@
         <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="P1" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="Q1" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S1" s="0" t="s">
         <v>18</v>
@@ -2901,16 +2898,16 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>14</v>
@@ -2919,19 +2916,19 @@
         <v>29</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K1" s="0" t="n">
         <v>12</v>
       </c>
       <c r="L1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>156</v>
       </c>
       <c r="O1" s="0" t="n">
         <v>5</v>
@@ -2946,13 +2943,13 @@
         <v>1</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V1" s="0" t="s">
         <v>18</v>
@@ -2999,7 +2996,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -3043,28 +3040,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3105,13 +3102,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3155,7 +3152,7 @@
         <v>30</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F1" s="11"/>
     </row>
@@ -3328,7 +3325,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3353,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3397,60 +3394,60 @@
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>35</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>1</v>
@@ -3494,10 +3491,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>29</v>

</xml_diff>